<commit_message>
update for week of 2/12
</commit_message>
<xml_diff>
--- a/Running Delta Smelt Catch_2023-09-05.xlsx
+++ b/Running Delta Smelt Catch_2023-09-05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp.sharepoint.com/sites/fws-FF08FBDT00-experimental-release-technical-team/Shared Documents/Recaptured fish data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/SmeltMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{759F0024-622B-46CF-8B91-4CAEF19DEE52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="6_{D7D8C1E3-0910-435B-88BC-04AB77536274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6A403506-1F7A-4636-BBFE-150CF9EBC122}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="12" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3433" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3472" uniqueCount="448">
   <si>
     <t>Running Delta Smelt Catch Data Collected for the USFWS Delta Smelt Experimental Release Technical Team</t>
   </si>
@@ -1398,13 +1398,19 @@
   </si>
   <si>
     <t>BY2023 4b</t>
+  </si>
+  <si>
+    <t>DJFMP</t>
+  </si>
+  <si>
+    <t>Efish</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1528,7 +1534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1612,48 +1618,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1998,18 +1967,18 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7265625" customWidth="1"/>
+    <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2020,7 +1989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2031,7 +2000,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -2042,7 +2011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -2050,7 +2019,7 @@
         <v>45272</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2058,7 +2027,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2066,7 +2035,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2074,7 +2043,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="12" t="s">
         <v>17</v>
       </c>
@@ -2096,7 +2065,7 @@
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>19</v>
       </c>
@@ -2104,7 +2073,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>21</v>
       </c>
@@ -2112,7 +2081,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>23</v>
       </c>
@@ -2120,7 +2089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
@@ -2128,7 +2097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>27</v>
       </c>
@@ -2136,27 +2105,27 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>33</v>
       </c>
@@ -2164,7 +2133,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>35</v>
       </c>
@@ -2172,7 +2141,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>37</v>
       </c>
@@ -2180,7 +2149,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>39</v>
       </c>
@@ -2188,7 +2157,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -2196,7 +2165,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -2204,7 +2173,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>45</v>
       </c>
@@ -2212,7 +2181,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -2220,7 +2189,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>49</v>
       </c>
@@ -2228,7 +2197,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="11" t="s">
         <v>51</v>
       </c>
@@ -2236,7 +2205,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="11" t="s">
         <v>53</v>
       </c>
@@ -2244,7 +2213,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="11" t="s">
         <v>55</v>
       </c>
@@ -2252,7 +2221,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="11" t="s">
         <v>57</v>
       </c>
@@ -2260,7 +2229,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="11" t="s">
         <v>59</v>
       </c>
@@ -2268,7 +2237,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="6" t="s">
         <v>61</v>
       </c>
@@ -2276,7 +2245,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="18" t="s">
         <v>63</v>
       </c>
@@ -2287,7 +2256,7 @@
       <c r="F41" s="18"/>
       <c r="G41" s="18"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="32" t="s">
         <v>64</v>
       </c>
@@ -2307,7 +2276,7 @@
       <c r="O44" s="12"/>
       <c r="P44" s="12"/>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="13">
         <v>45180</v>
       </c>
@@ -2315,7 +2284,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="13">
         <v>45251</v>
       </c>
@@ -2323,7 +2292,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="13">
         <v>45266</v>
       </c>
@@ -2342,39 +2311,40 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
-  <dimension ref="A1:AE238"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AE243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A213" sqref="A213:XFD238"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="35.140625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.28515625" style="14" customWidth="1"/>
-    <col min="12" max="13" width="14.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.453125" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.54296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="35.1796875" style="14" customWidth="1"/>
+    <col min="6" max="6" width="21.7265625" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.54296875" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.26953125" style="14" customWidth="1"/>
+    <col min="12" max="13" width="14.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.1796875" style="14" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19" style="14" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="26" style="14" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="43.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="31.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="43.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="31.81640625" style="14" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" style="14" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17.28515625" style="14" customWidth="1"/>
-    <col min="23" max="23" width="16.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.140625" style="23" customWidth="1"/>
+    <col min="21" max="22" width="17.26953125" style="14" customWidth="1"/>
+    <col min="23" max="23" width="16.26953125" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.1796875" style="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -2390,10 +2360,10 @@
       <c r="E1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="34" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="34" t="s">
         <v>30</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -2448,7 +2418,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>44546</v>
       </c>
@@ -2512,7 +2482,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>44547</v>
       </c>
@@ -2574,7 +2544,7 @@
       <c r="W3" s="19"/>
       <c r="X3" s="16"/>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>44547</v>
       </c>
@@ -2636,7 +2606,7 @@
       <c r="W4" s="19"/>
       <c r="X4" s="16"/>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>44547</v>
       </c>
@@ -2698,7 +2668,7 @@
       <c r="W5" s="19"/>
       <c r="X5" s="16"/>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>44547</v>
       </c>
@@ -2760,7 +2730,7 @@
       <c r="W6" s="19"/>
       <c r="X6" s="16"/>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>44547</v>
       </c>
@@ -2822,7 +2792,7 @@
       <c r="W7" s="19"/>
       <c r="X7" s="16"/>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>44547</v>
       </c>
@@ -2886,7 +2856,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>44547</v>
       </c>
@@ -2948,7 +2918,7 @@
       <c r="W9" s="19"/>
       <c r="X9" s="16"/>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>44551</v>
       </c>
@@ -3010,7 +2980,7 @@
       <c r="W10" s="19"/>
       <c r="X10" s="16"/>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>44553</v>
       </c>
@@ -3072,7 +3042,7 @@
       <c r="W11" s="19"/>
       <c r="X11" s="16"/>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>44553</v>
       </c>
@@ -3134,7 +3104,7 @@
       <c r="W12" s="19"/>
       <c r="X12" s="16"/>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="7">
         <v>44553</v>
       </c>
@@ -3196,7 +3166,7 @@
       <c r="W13" s="19"/>
       <c r="X13" s="16"/>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="7">
         <v>44557</v>
       </c>
@@ -3258,7 +3228,7 @@
       <c r="W14" s="19"/>
       <c r="X14" s="16"/>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="7">
         <v>44558</v>
       </c>
@@ -3320,7 +3290,7 @@
       <c r="W15" s="19"/>
       <c r="X15" s="16"/>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>44558</v>
       </c>
@@ -3382,7 +3352,7 @@
       <c r="W16" s="19"/>
       <c r="X16" s="16"/>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="7">
         <v>44559</v>
       </c>
@@ -3444,7 +3414,7 @@
       <c r="W17" s="19"/>
       <c r="X17" s="16"/>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="7">
         <v>44565</v>
       </c>
@@ -3460,10 +3430,10 @@
       <c r="E18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F18" s="47">
+      <c r="F18" s="35">
         <v>212</v>
       </c>
-      <c r="G18" s="47">
+      <c r="G18" s="35">
         <v>8</v>
       </c>
       <c r="H18" s="1"/>
@@ -3512,7 +3482,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="7">
         <v>44566</v>
       </c>
@@ -3576,7 +3546,7 @@
       </c>
       <c r="X19" s="16"/>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="7">
         <v>44573</v>
       </c>
@@ -3640,7 +3610,7 @@
       </c>
       <c r="X20" s="16"/>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A21" s="7">
         <v>44573</v>
       </c>
@@ -3704,7 +3674,7 @@
       </c>
       <c r="X21" s="16"/>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>44577</v>
       </c>
@@ -3770,7 +3740,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A23" s="7">
         <v>44579</v>
       </c>
@@ -3834,7 +3804,7 @@
       </c>
       <c r="X23" s="16"/>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A24" s="7">
         <v>44585</v>
       </c>
@@ -3898,7 +3868,7 @@
       </c>
       <c r="X24" s="16"/>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A25" s="7">
         <v>44592</v>
       </c>
@@ -3962,7 +3932,7 @@
       </c>
       <c r="X25" s="16"/>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A26" s="7">
         <v>44592</v>
       </c>
@@ -4026,7 +3996,7 @@
       </c>
       <c r="X26" s="16"/>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A27" s="7">
         <v>44596</v>
       </c>
@@ -4090,7 +4060,7 @@
       </c>
       <c r="X27" s="16"/>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A28" s="7">
         <v>44599</v>
       </c>
@@ -4154,7 +4124,7 @@
       </c>
       <c r="X28" s="16"/>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A29" s="7">
         <v>44606</v>
       </c>
@@ -4218,7 +4188,7 @@
       </c>
       <c r="X29" s="16"/>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A30" s="5">
         <v>44609</v>
       </c>
@@ -4234,10 +4204,10 @@
       <c r="E30" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F30" s="47">
+      <c r="F30" s="35">
         <v>181</v>
       </c>
-      <c r="G30" s="47">
+      <c r="G30" s="35">
         <v>9.5</v>
       </c>
       <c r="H30" s="1"/>
@@ -4288,7 +4258,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A31" s="7">
         <v>44609</v>
       </c>
@@ -4352,7 +4322,7 @@
       </c>
       <c r="X31" s="16"/>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>44610</v>
       </c>
@@ -4368,16 +4338,16 @@
       <c r="E32" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F32" s="48">
+      <c r="F32" s="35">
         <v>3893</v>
       </c>
-      <c r="G32" s="48">
+      <c r="G32" s="35">
         <v>11.8</v>
       </c>
-      <c r="H32" s="45">
+      <c r="H32" s="6">
         <v>56.4</v>
       </c>
-      <c r="I32" s="45" t="s">
+      <c r="I32" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J32" s="1">
@@ -4424,7 +4394,7 @@
       </c>
       <c r="X32" s="16"/>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>44610</v>
       </c>
@@ -4440,16 +4410,16 @@
       <c r="E33" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F33" s="48">
+      <c r="F33" s="35">
         <v>3893</v>
       </c>
-      <c r="G33" s="48">
+      <c r="G33" s="35">
         <v>11.8</v>
       </c>
-      <c r="H33" s="45">
+      <c r="H33" s="6">
         <v>56.4</v>
       </c>
-      <c r="I33" s="45" t="s">
+      <c r="I33" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J33" s="1">
@@ -4496,7 +4466,7 @@
       </c>
       <c r="X33" s="16"/>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>44610</v>
       </c>
@@ -4512,16 +4482,16 @@
       <c r="E34" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F34" s="48">
+      <c r="F34" s="35">
         <v>3893</v>
       </c>
-      <c r="G34" s="48">
+      <c r="G34" s="35">
         <v>11.8</v>
       </c>
-      <c r="H34" s="45">
+      <c r="H34" s="6">
         <v>56.4</v>
       </c>
-      <c r="I34" s="45" t="s">
+      <c r="I34" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J34" s="1">
@@ -4568,7 +4538,7 @@
       </c>
       <c r="X34" s="16"/>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>44610</v>
       </c>
@@ -4584,16 +4554,16 @@
       <c r="E35" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F35" s="48">
+      <c r="F35" s="35">
         <v>3893</v>
       </c>
-      <c r="G35" s="48">
+      <c r="G35" s="35">
         <v>11.8</v>
       </c>
-      <c r="H35" s="45">
+      <c r="H35" s="6">
         <v>56.4</v>
       </c>
-      <c r="I35" s="45" t="s">
+      <c r="I35" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J35" s="1">
@@ -4640,7 +4610,7 @@
       </c>
       <c r="X35" s="16"/>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>44610</v>
       </c>
@@ -4656,16 +4626,16 @@
       <c r="E36" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F36" s="48">
+      <c r="F36" s="35">
         <v>3427</v>
       </c>
-      <c r="G36" s="48">
+      <c r="G36" s="35">
         <v>11.2</v>
       </c>
-      <c r="H36" s="45">
+      <c r="H36" s="6">
         <v>38.9</v>
       </c>
-      <c r="I36" s="45" t="s">
+      <c r="I36" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J36" s="1">
@@ -4712,7 +4682,7 @@
       </c>
       <c r="X36" s="16"/>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A37" s="7">
         <v>44615</v>
       </c>
@@ -4776,7 +4746,7 @@
       </c>
       <c r="X37" s="16"/>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="7">
         <v>44615</v>
       </c>
@@ -4840,7 +4810,7 @@
       </c>
       <c r="X38" s="16"/>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="7">
         <v>44615</v>
       </c>
@@ -4904,7 +4874,7 @@
       </c>
       <c r="X39" s="16"/>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="7">
         <v>44615</v>
       </c>
@@ -4968,7 +4938,7 @@
       </c>
       <c r="X40" s="16"/>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="7">
         <v>44615</v>
       </c>
@@ -5032,7 +5002,7 @@
       </c>
       <c r="X41" s="16"/>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A42" s="7">
         <v>44616</v>
       </c>
@@ -5096,7 +5066,7 @@
       </c>
       <c r="X42" s="16"/>
     </row>
-    <row r="43" spans="1:24">
+    <row r="43" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="7">
         <v>44616</v>
       </c>
@@ -5160,7 +5130,7 @@
       </c>
       <c r="X43" s="16"/>
     </row>
-    <row r="44" spans="1:24">
+    <row r="44" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="7">
         <v>44616</v>
       </c>
@@ -5224,7 +5194,7 @@
       </c>
       <c r="X44" s="16"/>
     </row>
-    <row r="45" spans="1:24">
+    <row r="45" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="7">
         <v>44616</v>
       </c>
@@ -5288,7 +5258,7 @@
       </c>
       <c r="X45" s="16"/>
     </row>
-    <row r="46" spans="1:24">
+    <row r="46" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="7">
         <v>44622</v>
       </c>
@@ -5352,7 +5322,7 @@
       </c>
       <c r="X46" s="16"/>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="7">
         <v>44622</v>
       </c>
@@ -5416,7 +5386,7 @@
       </c>
       <c r="X47" s="16"/>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="7">
         <v>44622</v>
       </c>
@@ -5480,7 +5450,7 @@
       </c>
       <c r="X48" s="16"/>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="7">
         <v>44622</v>
       </c>
@@ -5544,7 +5514,7 @@
       </c>
       <c r="X49" s="16"/>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="7">
         <v>44623</v>
       </c>
@@ -5608,7 +5578,7 @@
       </c>
       <c r="X50" s="16"/>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A51" s="7">
         <v>44628</v>
       </c>
@@ -5672,7 +5642,7 @@
       </c>
       <c r="X51" s="16"/>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A52" s="7">
         <v>44628</v>
       </c>
@@ -5736,7 +5706,7 @@
       </c>
       <c r="X52" s="16"/>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A53" s="7">
         <v>44628</v>
       </c>
@@ -5800,7 +5770,7 @@
       </c>
       <c r="X53" s="16"/>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A54" s="7">
         <v>44628</v>
       </c>
@@ -5864,7 +5834,7 @@
       </c>
       <c r="X54" s="16"/>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A55" s="7">
         <v>44628</v>
       </c>
@@ -5928,7 +5898,7 @@
       </c>
       <c r="X55" s="16"/>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A56" s="7">
         <v>44631</v>
       </c>
@@ -5992,7 +5962,7 @@
       </c>
       <c r="X56" s="16"/>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A57" s="7">
         <v>44631</v>
       </c>
@@ -6056,7 +6026,7 @@
       </c>
       <c r="X57" s="16"/>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>44636</v>
       </c>
@@ -6072,16 +6042,16 @@
       <c r="E58" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F58" s="48">
+      <c r="F58" s="35">
         <v>348</v>
       </c>
-      <c r="G58" s="48">
+      <c r="G58" s="35">
         <v>13.7</v>
       </c>
-      <c r="H58" s="45">
+      <c r="H58" s="6">
         <v>44.1</v>
       </c>
-      <c r="I58" s="45" t="s">
+      <c r="I58" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J58" s="1">
@@ -6128,7 +6098,7 @@
       </c>
       <c r="X58" s="16"/>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>44636</v>
       </c>
@@ -6144,16 +6114,16 @@
       <c r="E59" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F59" s="48">
+      <c r="F59" s="35">
         <v>348</v>
       </c>
-      <c r="G59" s="48">
+      <c r="G59" s="35">
         <v>13.7</v>
       </c>
-      <c r="H59" s="45">
+      <c r="H59" s="6">
         <v>44.1</v>
       </c>
-      <c r="I59" s="45" t="s">
+      <c r="I59" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J59" s="1">
@@ -6200,7 +6170,7 @@
       </c>
       <c r="X59" s="16"/>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A60" s="5">
         <v>44636</v>
       </c>
@@ -6216,16 +6186,16 @@
       <c r="E60" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F60" s="48">
+      <c r="F60" s="35">
         <v>340</v>
       </c>
-      <c r="G60" s="48">
+      <c r="G60" s="35">
         <v>13.2</v>
       </c>
-      <c r="H60" s="45">
+      <c r="H60" s="6">
         <v>18.5</v>
       </c>
-      <c r="I60" s="45" t="s">
+      <c r="I60" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J60" s="1">
@@ -6272,7 +6242,7 @@
       </c>
       <c r="X60" s="16"/>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A61" s="7">
         <v>44637</v>
       </c>
@@ -6336,7 +6306,7 @@
       </c>
       <c r="X61" s="16"/>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>44637</v>
       </c>
@@ -6352,16 +6322,16 @@
       <c r="E62" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F62" s="48">
+      <c r="F62" s="35">
         <v>3608</v>
       </c>
-      <c r="G62" s="48">
+      <c r="G62" s="35">
         <v>14</v>
       </c>
-      <c r="H62" s="45">
+      <c r="H62" s="6">
         <v>67.599999999999994</v>
       </c>
-      <c r="I62" s="45" t="s">
+      <c r="I62" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J62" s="1">
@@ -6408,7 +6378,7 @@
       </c>
       <c r="X62" s="16"/>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>44637</v>
       </c>
@@ -6424,16 +6394,16 @@
       <c r="E63" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F63" s="48">
+      <c r="F63" s="35">
         <v>3608</v>
       </c>
-      <c r="G63" s="48">
+      <c r="G63" s="35">
         <v>14</v>
       </c>
-      <c r="H63" s="45">
+      <c r="H63" s="6">
         <v>67.599999999999994</v>
       </c>
-      <c r="I63" s="45" t="s">
+      <c r="I63" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J63" s="1">
@@ -6480,7 +6450,7 @@
       </c>
       <c r="X63" s="16"/>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>44637</v>
       </c>
@@ -6496,16 +6466,16 @@
       <c r="E64" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F64" s="48">
+      <c r="F64" s="35">
         <v>3608</v>
       </c>
-      <c r="G64" s="48">
+      <c r="G64" s="35">
         <v>14</v>
       </c>
-      <c r="H64" s="45">
+      <c r="H64" s="6">
         <v>67.599999999999994</v>
       </c>
-      <c r="I64" s="45" t="s">
+      <c r="I64" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J64" s="1">
@@ -6552,7 +6522,7 @@
       </c>
       <c r="X64" s="16"/>
     </row>
-    <row r="65" spans="1:24">
+    <row r="65" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>44637</v>
       </c>
@@ -6568,16 +6538,16 @@
       <c r="E65" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F65" s="48">
+      <c r="F65" s="35">
         <v>3608</v>
       </c>
-      <c r="G65" s="48">
+      <c r="G65" s="35">
         <v>14</v>
       </c>
-      <c r="H65" s="45">
+      <c r="H65" s="6">
         <v>67.599999999999994</v>
       </c>
-      <c r="I65" s="45" t="s">
+      <c r="I65" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J65" s="1">
@@ -6624,7 +6594,7 @@
       </c>
       <c r="X65" s="16"/>
     </row>
-    <row r="66" spans="1:24">
+    <row r="66" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>44637</v>
       </c>
@@ -6640,16 +6610,16 @@
       <c r="E66" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F66" s="48">
+      <c r="F66" s="35">
         <v>2163</v>
       </c>
-      <c r="G66" s="48">
+      <c r="G66" s="35">
         <v>14.5</v>
       </c>
-      <c r="H66" s="45">
+      <c r="H66" s="6">
         <v>56.7</v>
       </c>
-      <c r="I66" s="45" t="s">
+      <c r="I66" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J66" s="1">
@@ -6696,7 +6666,7 @@
       </c>
       <c r="X66" s="16"/>
     </row>
-    <row r="67" spans="1:24">
+    <row r="67" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>44637</v>
       </c>
@@ -6712,16 +6682,16 @@
       <c r="E67" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F67" s="48">
+      <c r="F67" s="35">
         <v>2163</v>
       </c>
-      <c r="G67" s="48">
+      <c r="G67" s="35">
         <v>14.5</v>
       </c>
-      <c r="H67" s="45">
+      <c r="H67" s="6">
         <v>56.7</v>
       </c>
-      <c r="I67" s="45" t="s">
+      <c r="I67" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J67" s="1">
@@ -6768,7 +6738,7 @@
       </c>
       <c r="X67" s="16"/>
     </row>
-    <row r="68" spans="1:24">
+    <row r="68" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>44637</v>
       </c>
@@ -6784,16 +6754,16 @@
       <c r="E68" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F68" s="48">
+      <c r="F68" s="35">
         <v>2163</v>
       </c>
-      <c r="G68" s="48">
+      <c r="G68" s="35">
         <v>14.5</v>
       </c>
-      <c r="H68" s="45">
+      <c r="H68" s="6">
         <v>56.7</v>
       </c>
-      <c r="I68" s="45" t="s">
+      <c r="I68" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J68" s="1">
@@ -6840,7 +6810,7 @@
       </c>
       <c r="X68" s="16"/>
     </row>
-    <row r="69" spans="1:24">
+    <row r="69" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>44637</v>
       </c>
@@ -6856,16 +6826,16 @@
       <c r="E69" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F69" s="48">
+      <c r="F69" s="35">
         <v>2163</v>
       </c>
-      <c r="G69" s="48">
+      <c r="G69" s="35">
         <v>14.5</v>
       </c>
-      <c r="H69" s="45">
+      <c r="H69" s="6">
         <v>56.7</v>
       </c>
-      <c r="I69" s="45" t="s">
+      <c r="I69" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J69" s="1">
@@ -6912,7 +6882,7 @@
       </c>
       <c r="X69" s="16"/>
     </row>
-    <row r="70" spans="1:24">
+    <row r="70" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A70" s="7">
         <v>44641</v>
       </c>
@@ -6976,7 +6946,7 @@
       </c>
       <c r="X70" s="16"/>
     </row>
-    <row r="71" spans="1:24">
+    <row r="71" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="5">
         <v>44641</v>
       </c>
@@ -6992,16 +6962,16 @@
       <c r="E71" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F71" s="48">
+      <c r="F71" s="35">
         <v>438</v>
       </c>
-      <c r="G71" s="48">
+      <c r="G71" s="35">
         <v>14.5</v>
       </c>
-      <c r="H71" s="45">
+      <c r="H71" s="6">
         <v>26.3</v>
       </c>
-      <c r="I71" s="45" t="s">
+      <c r="I71" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J71" s="1">
@@ -7048,7 +7018,7 @@
       </c>
       <c r="X71" s="16"/>
     </row>
-    <row r="72" spans="1:24">
+    <row r="72" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="5">
         <v>44641</v>
       </c>
@@ -7064,16 +7034,16 @@
       <c r="E72" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F72" s="48">
+      <c r="F72" s="35">
         <v>438</v>
       </c>
-      <c r="G72" s="48">
+      <c r="G72" s="35">
         <v>14.5</v>
       </c>
-      <c r="H72" s="45">
+      <c r="H72" s="6">
         <v>26.3</v>
       </c>
-      <c r="I72" s="45" t="s">
+      <c r="I72" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J72" s="1">
@@ -7120,7 +7090,7 @@
       </c>
       <c r="X72" s="16"/>
     </row>
-    <row r="73" spans="1:24">
+    <row r="73" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="5">
         <v>44641</v>
       </c>
@@ -7136,16 +7106,16 @@
       <c r="E73" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F73" s="48">
+      <c r="F73" s="35">
         <v>272</v>
       </c>
-      <c r="G73" s="48">
+      <c r="G73" s="35">
         <v>14.1</v>
       </c>
-      <c r="H73" s="45">
+      <c r="H73" s="6">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I73" s="45" t="s">
+      <c r="I73" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J73" s="1">
@@ -7192,7 +7162,7 @@
       </c>
       <c r="X73" s="16"/>
     </row>
-    <row r="74" spans="1:24">
+    <row r="74" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="5">
         <v>44641</v>
       </c>
@@ -7208,16 +7178,16 @@
       <c r="E74" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F74" s="48">
+      <c r="F74" s="35">
         <v>205</v>
       </c>
-      <c r="G74" s="48">
+      <c r="G74" s="35">
         <v>14.1</v>
       </c>
-      <c r="H74" s="45">
+      <c r="H74" s="6">
         <v>4.5999999999999996</v>
       </c>
-      <c r="I74" s="45" t="s">
+      <c r="I74" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J74" s="1">
@@ -7264,7 +7234,7 @@
       </c>
       <c r="X74" s="16"/>
     </row>
-    <row r="75" spans="1:24">
+    <row r="75" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="5">
         <v>44641</v>
       </c>
@@ -7280,16 +7250,16 @@
       <c r="E75" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F75" s="48">
+      <c r="F75" s="35">
         <v>205</v>
       </c>
-      <c r="G75" s="48">
+      <c r="G75" s="35">
         <v>14.1</v>
       </c>
-      <c r="H75" s="45">
+      <c r="H75" s="6">
         <v>4.5999999999999996</v>
       </c>
-      <c r="I75" s="45" t="s">
+      <c r="I75" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J75" s="1">
@@ -7336,7 +7306,7 @@
       </c>
       <c r="X75" s="16"/>
     </row>
-    <row r="76" spans="1:24">
+    <row r="76" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="5">
         <v>44641</v>
       </c>
@@ -7352,16 +7322,16 @@
       <c r="E76" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F76" s="48">
+      <c r="F76" s="35">
         <v>188</v>
       </c>
-      <c r="G76" s="48">
+      <c r="G76" s="35">
         <v>16.399999999999999</v>
       </c>
-      <c r="H76" s="45">
+      <c r="H76" s="6">
         <v>3.7</v>
       </c>
-      <c r="I76" s="45" t="s">
+      <c r="I76" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J76" s="1">
@@ -7408,7 +7378,7 @@
       </c>
       <c r="X76" s="16"/>
     </row>
-    <row r="77" spans="1:24">
+    <row r="77" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A77" s="7">
         <v>44642</v>
       </c>
@@ -7472,7 +7442,7 @@
       </c>
       <c r="X77" s="16"/>
     </row>
-    <row r="78" spans="1:24">
+    <row r="78" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A78" s="7">
         <v>44643</v>
       </c>
@@ -7536,7 +7506,7 @@
       </c>
       <c r="X78" s="16"/>
     </row>
-    <row r="79" spans="1:24">
+    <row r="79" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A79" s="7">
         <v>44643</v>
       </c>
@@ -7600,7 +7570,7 @@
       </c>
       <c r="X79" s="16"/>
     </row>
-    <row r="80" spans="1:24">
+    <row r="80" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A80" s="7">
         <v>44643</v>
       </c>
@@ -7664,7 +7634,7 @@
       </c>
       <c r="X80" s="16"/>
     </row>
-    <row r="81" spans="1:24">
+    <row r="81" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A81" s="7">
         <v>44643</v>
       </c>
@@ -7728,7 +7698,7 @@
       </c>
       <c r="X81" s="16"/>
     </row>
-    <row r="82" spans="1:24">
+    <row r="82" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A82" s="7">
         <v>44643</v>
       </c>
@@ -7792,7 +7762,7 @@
       </c>
       <c r="X82" s="16"/>
     </row>
-    <row r="83" spans="1:24">
+    <row r="83" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A83" s="7">
         <v>44643</v>
       </c>
@@ -7856,7 +7826,7 @@
       </c>
       <c r="X83" s="16"/>
     </row>
-    <row r="84" spans="1:24">
+    <row r="84" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="5">
         <v>44643</v>
       </c>
@@ -7872,16 +7842,16 @@
       <c r="E84" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F84" s="48">
+      <c r="F84" s="35">
         <v>183</v>
       </c>
-      <c r="G84" s="48">
+      <c r="G84" s="35">
         <v>15.3</v>
       </c>
-      <c r="H84" s="45">
+      <c r="H84" s="6">
         <v>5.7</v>
       </c>
-      <c r="I84" s="45" t="s">
+      <c r="I84" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J84" s="1">
@@ -7928,7 +7898,7 @@
       </c>
       <c r="X84" s="16"/>
     </row>
-    <row r="85" spans="1:24">
+    <row r="85" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="5">
         <v>44643</v>
       </c>
@@ -7944,16 +7914,16 @@
       <c r="E85" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F85" s="48">
+      <c r="F85" s="35">
         <v>183</v>
       </c>
-      <c r="G85" s="48">
+      <c r="G85" s="35">
         <v>15.3</v>
       </c>
-      <c r="H85" s="45">
+      <c r="H85" s="6">
         <v>5.7</v>
       </c>
-      <c r="I85" s="45" t="s">
+      <c r="I85" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J85" s="1">
@@ -8000,7 +7970,7 @@
       </c>
       <c r="X85" s="16"/>
     </row>
-    <row r="86" spans="1:24">
+    <row r="86" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A86" s="7">
         <v>44649</v>
       </c>
@@ -8064,7 +8034,7 @@
       </c>
       <c r="X86" s="16"/>
     </row>
-    <row r="87" spans="1:24">
+    <row r="87" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A87" s="7">
         <v>44651</v>
       </c>
@@ -8128,7 +8098,7 @@
       </c>
       <c r="X87" s="16"/>
     </row>
-    <row r="88" spans="1:24">
+    <row r="88" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="7">
         <v>44656</v>
       </c>
@@ -8192,7 +8162,7 @@
       </c>
       <c r="X88" s="16"/>
     </row>
-    <row r="89" spans="1:24">
+    <row r="89" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="7">
         <v>44656</v>
       </c>
@@ -8256,7 +8226,7 @@
       </c>
       <c r="X89" s="16"/>
     </row>
-    <row r="90" spans="1:24">
+    <row r="90" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="7">
         <v>44656</v>
       </c>
@@ -8320,7 +8290,7 @@
       </c>
       <c r="X90" s="16"/>
     </row>
-    <row r="91" spans="1:24">
+    <row r="91" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="5">
         <v>44656</v>
       </c>
@@ -8336,16 +8306,16 @@
       <c r="E91" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="F91" s="48">
+      <c r="F91" s="35">
         <v>314</v>
       </c>
-      <c r="G91" s="48">
+      <c r="G91" s="35">
         <v>15.8</v>
       </c>
-      <c r="H91" s="45">
+      <c r="H91" s="6">
         <v>7.7</v>
       </c>
-      <c r="I91" s="45" t="s">
+      <c r="I91" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J91" s="1">
@@ -8392,7 +8362,7 @@
       </c>
       <c r="X91" s="16"/>
     </row>
-    <row r="92" spans="1:24">
+    <row r="92" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="5">
         <v>44658</v>
       </c>
@@ -8408,16 +8378,16 @@
       <c r="E92" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F92" s="48">
+      <c r="F92" s="35">
         <v>164</v>
       </c>
-      <c r="G92" s="48">
+      <c r="G92" s="35">
         <v>18</v>
       </c>
-      <c r="H92" s="45">
+      <c r="H92" s="6">
         <v>3.5</v>
       </c>
-      <c r="I92" s="45" t="s">
+      <c r="I92" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J92" s="1">
@@ -8464,7 +8434,7 @@
       </c>
       <c r="X92" s="16"/>
     </row>
-    <row r="93" spans="1:24">
+    <row r="93" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="5">
         <v>44664</v>
       </c>
@@ -8480,16 +8450,16 @@
       <c r="E93" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F93" s="48">
+      <c r="F93" s="35">
         <v>421</v>
       </c>
-      <c r="G93" s="48">
+      <c r="G93" s="35">
         <v>15.8</v>
       </c>
-      <c r="H93" s="45">
+      <c r="H93" s="6">
         <v>13.3</v>
       </c>
-      <c r="I93" s="45" t="s">
+      <c r="I93" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J93" s="1">
@@ -8536,7 +8506,7 @@
       </c>
       <c r="X93" s="16"/>
     </row>
-    <row r="94" spans="1:24">
+    <row r="94" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="5">
         <v>44665</v>
       </c>
@@ -8552,16 +8522,16 @@
       <c r="E94" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F94" s="48">
+      <c r="F94" s="35">
         <v>4435</v>
       </c>
-      <c r="G94" s="48">
+      <c r="G94" s="35">
         <v>15.3</v>
       </c>
-      <c r="H94" s="45">
+      <c r="H94" s="6">
         <v>49.3</v>
       </c>
-      <c r="I94" s="45" t="s">
+      <c r="I94" s="6" t="s">
         <v>155</v>
       </c>
       <c r="J94" s="1">
@@ -8608,7 +8578,7 @@
       </c>
       <c r="X94" s="16"/>
     </row>
-    <row r="95" spans="1:24">
+    <row r="95" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="7">
         <v>44669</v>
       </c>
@@ -8672,7 +8642,7 @@
       </c>
       <c r="X95" s="16"/>
     </row>
-    <row r="96" spans="1:24">
+    <row r="96" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="7">
         <v>44669</v>
       </c>
@@ -8736,7 +8706,7 @@
       </c>
       <c r="X96" s="16"/>
     </row>
-    <row r="97" spans="1:24">
+    <row r="97" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="7">
         <v>44669</v>
       </c>
@@ -8800,7 +8770,7 @@
       </c>
       <c r="X97" s="16"/>
     </row>
-    <row r="98" spans="1:24">
+    <row r="98" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="7">
         <v>44669</v>
       </c>
@@ -8864,7 +8834,7 @@
       </c>
       <c r="X98" s="16"/>
     </row>
-    <row r="99" spans="1:24">
+    <row r="99" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="7">
         <v>44673</v>
       </c>
@@ -8928,7 +8898,7 @@
       </c>
       <c r="X99" s="16"/>
     </row>
-    <row r="100" spans="1:24">
+    <row r="100" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="7">
         <v>44684</v>
       </c>
@@ -8992,7 +8962,7 @@
       </c>
       <c r="X100" s="16"/>
     </row>
-    <row r="101" spans="1:24">
+    <row r="101" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="7">
         <v>44684</v>
       </c>
@@ -9056,7 +9026,7 @@
       </c>
       <c r="X101" s="16"/>
     </row>
-    <row r="102" spans="1:24">
+    <row r="102" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="7">
         <v>44684</v>
       </c>
@@ -9120,7 +9090,7 @@
       </c>
       <c r="X102" s="16"/>
     </row>
-    <row r="103" spans="1:24">
+    <row r="103" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="7">
         <v>44690</v>
       </c>
@@ -9184,7 +9154,7 @@
       </c>
       <c r="X103" s="16"/>
     </row>
-    <row r="104" spans="1:24">
+    <row r="104" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="7">
         <v>44690</v>
       </c>
@@ -9248,7 +9218,7 @@
       </c>
       <c r="X104" s="16"/>
     </row>
-    <row r="105" spans="1:24">
+    <row r="105" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="7">
         <v>44691</v>
       </c>
@@ -9312,7 +9282,7 @@
       </c>
       <c r="X105" s="16"/>
     </row>
-    <row r="106" spans="1:24">
+    <row r="106" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="7">
         <v>44691</v>
       </c>
@@ -9376,7 +9346,7 @@
       </c>
       <c r="X106" s="16"/>
     </row>
-    <row r="107" spans="1:24">
+    <row r="107" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="7">
         <v>44691</v>
       </c>
@@ -9440,7 +9410,7 @@
       </c>
       <c r="X107" s="16"/>
     </row>
-    <row r="108" spans="1:24">
+    <row r="108" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="7">
         <v>44691</v>
       </c>
@@ -9504,7 +9474,7 @@
       </c>
       <c r="X108" s="16"/>
     </row>
-    <row r="109" spans="1:24">
+    <row r="109" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="7">
         <v>44713</v>
       </c>
@@ -9568,7 +9538,7 @@
       </c>
       <c r="X109" s="16"/>
     </row>
-    <row r="110" spans="1:24">
+    <row r="110" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="7">
         <v>44718</v>
       </c>
@@ -9632,7 +9602,7 @@
       </c>
       <c r="X110" s="16"/>
     </row>
-    <row r="111" spans="1:24">
+    <row r="111" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="7">
         <v>44775</v>
       </c>
@@ -9696,7 +9666,7 @@
       </c>
       <c r="X111" s="16"/>
     </row>
-    <row r="112" spans="1:24">
+    <row r="112" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="7">
         <v>44775</v>
       </c>
@@ -9760,7 +9730,7 @@
       </c>
       <c r="X112" s="16"/>
     </row>
-    <row r="113" spans="1:24">
+    <row r="113" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="7">
         <v>44783</v>
       </c>
@@ -9824,7 +9794,7 @@
       </c>
       <c r="X113" s="16"/>
     </row>
-    <row r="114" spans="1:24">
+    <row r="114" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="7">
         <v>44788</v>
       </c>
@@ -9888,7 +9858,7 @@
       </c>
       <c r="X114" s="16"/>
     </row>
-    <row r="115" spans="1:24">
+    <row r="115" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115" s="7">
         <v>44789</v>
       </c>
@@ -9952,7 +9922,7 @@
       </c>
       <c r="X115" s="16"/>
     </row>
-    <row r="116" spans="1:24">
+    <row r="116" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="7">
         <v>44825</v>
       </c>
@@ -10016,7 +9986,7 @@
       </c>
       <c r="X116" s="16"/>
     </row>
-    <row r="117" spans="1:24">
+    <row r="117" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="7">
         <v>44868</v>
       </c>
@@ -10082,7 +10052,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="118" spans="1:24">
+    <row r="118" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="7">
         <v>44872</v>
       </c>
@@ -10148,7 +10118,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="119" spans="1:24">
+    <row r="119" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A119" s="5">
         <v>44909</v>
       </c>
@@ -10214,7 +10184,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="120" spans="1:24">
+    <row r="120" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" s="5">
         <v>44909</v>
       </c>
@@ -10280,7 +10250,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="121" spans="1:24">
+    <row r="121" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A121" s="5">
         <v>44933</v>
       </c>
@@ -10344,7 +10314,7 @@
       </c>
       <c r="X121" s="16"/>
     </row>
-    <row r="122" spans="1:24">
+    <row r="122" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122" s="7">
         <v>44943</v>
       </c>
@@ -10408,7 +10378,7 @@
       </c>
       <c r="X122" s="16"/>
     </row>
-    <row r="123" spans="1:24">
+    <row r="123" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A123" s="7">
         <v>44945</v>
       </c>
@@ -10472,7 +10442,7 @@
       </c>
       <c r="X123" s="16"/>
     </row>
-    <row r="124" spans="1:24">
+    <row r="124" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A124" s="7">
         <v>44950</v>
       </c>
@@ -10538,7 +10508,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="125" spans="1:24">
+    <row r="125" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A125" s="7">
         <v>44952</v>
       </c>
@@ -10602,7 +10572,7 @@
       </c>
       <c r="X125" s="16"/>
     </row>
-    <row r="126" spans="1:24">
+    <row r="126" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A126" s="7">
         <v>44953</v>
       </c>
@@ -10666,7 +10636,7 @@
       </c>
       <c r="X126" s="16"/>
     </row>
-    <row r="127" spans="1:24">
+    <row r="127" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A127" s="7">
         <v>44956</v>
       </c>
@@ -10730,7 +10700,7 @@
       </c>
       <c r="X127" s="16"/>
     </row>
-    <row r="128" spans="1:24">
+    <row r="128" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A128" s="7">
         <v>44956</v>
       </c>
@@ -10794,7 +10764,7 @@
       </c>
       <c r="X128" s="16"/>
     </row>
-    <row r="129" spans="1:24">
+    <row r="129" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A129" s="7">
         <v>44956</v>
       </c>
@@ -10858,7 +10828,7 @@
       </c>
       <c r="X129" s="16"/>
     </row>
-    <row r="130" spans="1:24">
+    <row r="130" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A130" s="7">
         <v>44957</v>
       </c>
@@ -10922,7 +10892,7 @@
       </c>
       <c r="X130" s="16"/>
     </row>
-    <row r="131" spans="1:24">
+    <row r="131" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="7">
         <v>44957</v>
       </c>
@@ -10986,7 +10956,7 @@
       </c>
       <c r="X131" s="16"/>
     </row>
-    <row r="132" spans="1:24">
+    <row r="132" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A132" s="7">
         <v>44958</v>
       </c>
@@ -11050,7 +11020,7 @@
       </c>
       <c r="X132" s="16"/>
     </row>
-    <row r="133" spans="1:24">
+    <row r="133" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A133" s="7">
         <v>44958</v>
       </c>
@@ -11114,7 +11084,7 @@
       </c>
       <c r="X133" s="16"/>
     </row>
-    <row r="134" spans="1:24">
+    <row r="134" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A134" s="7">
         <v>44958</v>
       </c>
@@ -11178,7 +11148,7 @@
       </c>
       <c r="X134" s="16"/>
     </row>
-    <row r="135" spans="1:24">
+    <row r="135" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A135" s="7">
         <v>44958</v>
       </c>
@@ -11242,7 +11212,7 @@
       </c>
       <c r="X135" s="16"/>
     </row>
-    <row r="136" spans="1:24">
+    <row r="136" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A136" s="7">
         <v>44959</v>
       </c>
@@ -11306,7 +11276,7 @@
       </c>
       <c r="X136" s="16"/>
     </row>
-    <row r="137" spans="1:24">
+    <row r="137" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A137" s="7">
         <v>44960</v>
       </c>
@@ -11370,7 +11340,7 @@
       </c>
       <c r="X137" s="16"/>
     </row>
-    <row r="138" spans="1:24">
+    <row r="138" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A138" s="7">
         <v>44960</v>
       </c>
@@ -11434,7 +11404,7 @@
       </c>
       <c r="X138" s="16"/>
     </row>
-    <row r="139" spans="1:24">
+    <row r="139" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A139" s="7">
         <v>44960</v>
       </c>
@@ -11498,7 +11468,7 @@
       </c>
       <c r="X139" s="16"/>
     </row>
-    <row r="140" spans="1:24">
+    <row r="140" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A140" s="7">
         <v>44964</v>
       </c>
@@ -11562,7 +11532,7 @@
       </c>
       <c r="X140" s="16"/>
     </row>
-    <row r="141" spans="1:24">
+    <row r="141" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A141" s="5">
         <v>44965</v>
       </c>
@@ -11578,16 +11548,16 @@
       <c r="E141" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F141" s="48">
+      <c r="F141" s="35">
         <v>588</v>
       </c>
-      <c r="G141" s="48">
+      <c r="G141" s="35">
         <v>9.3000000000000007</v>
       </c>
-      <c r="H141" s="45">
+      <c r="H141" s="6">
         <v>52.5</v>
       </c>
-      <c r="I141" s="45">
+      <c r="I141" s="6">
         <v>36.9</v>
       </c>
       <c r="J141" s="1">
@@ -11634,7 +11604,7 @@
       </c>
       <c r="X141" s="16"/>
     </row>
-    <row r="142" spans="1:24">
+    <row r="142" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A142" s="5">
         <v>44965</v>
       </c>
@@ -11650,16 +11620,16 @@
       <c r="E142" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F142" s="48">
+      <c r="F142" s="35">
         <v>242</v>
       </c>
-      <c r="G142" s="48">
+      <c r="G142" s="35">
         <v>8.5</v>
       </c>
-      <c r="H142" s="45">
+      <c r="H142" s="6">
         <v>25.3</v>
       </c>
-      <c r="I142" s="45">
+      <c r="I142" s="6">
         <v>19.2</v>
       </c>
       <c r="J142" s="1">
@@ -11706,7 +11676,7 @@
       </c>
       <c r="X142" s="16"/>
     </row>
-    <row r="143" spans="1:24">
+    <row r="143" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A143" s="5">
         <v>44965</v>
       </c>
@@ -11770,7 +11740,7 @@
       </c>
       <c r="X143" s="16"/>
     </row>
-    <row r="144" spans="1:24">
+    <row r="144" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="7">
         <v>44966</v>
       </c>
@@ -11836,7 +11806,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="145" spans="1:24">
+    <row r="145" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A145" s="5">
         <v>44969</v>
       </c>
@@ -11900,7 +11870,7 @@
       </c>
       <c r="X145" s="16"/>
     </row>
-    <row r="146" spans="1:24">
+    <row r="146" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A146" s="5">
         <v>44970</v>
       </c>
@@ -11964,7 +11934,7 @@
       </c>
       <c r="X146" s="16"/>
     </row>
-    <row r="147" spans="1:24">
+    <row r="147" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A147" s="5">
         <v>44970</v>
       </c>
@@ -12028,7 +11998,7 @@
       </c>
       <c r="X147" s="16"/>
     </row>
-    <row r="148" spans="1:24">
+    <row r="148" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A148" s="7">
         <v>44971</v>
       </c>
@@ -12092,7 +12062,7 @@
       </c>
       <c r="X148" s="16"/>
     </row>
-    <row r="149" spans="1:24">
+    <row r="149" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A149" s="5">
         <v>44971</v>
       </c>
@@ -12156,7 +12126,7 @@
       </c>
       <c r="X149" s="16"/>
     </row>
-    <row r="150" spans="1:24">
+    <row r="150" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A150" s="7">
         <v>44972</v>
       </c>
@@ -12220,7 +12190,7 @@
       </c>
       <c r="X150" s="16"/>
     </row>
-    <row r="151" spans="1:24">
+    <row r="151" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A151" s="7">
         <v>44974</v>
       </c>
@@ -12284,7 +12254,7 @@
       </c>
       <c r="X151" s="16"/>
     </row>
-    <row r="152" spans="1:24">
+    <row r="152" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A152" s="5">
         <v>44974</v>
       </c>
@@ -12348,7 +12318,7 @@
       </c>
       <c r="X152" s="16"/>
     </row>
-    <row r="153" spans="1:24" s="18" customFormat="1">
+    <row r="153" spans="1:24" s="18" customFormat="1" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A153" s="28">
         <v>44975</v>
       </c>
@@ -12414,7 +12384,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="154" spans="1:24">
+    <row r="154" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A154" s="7">
         <v>44976</v>
       </c>
@@ -12478,7 +12448,7 @@
       </c>
       <c r="X154" s="16"/>
     </row>
-    <row r="155" spans="1:24">
+    <row r="155" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A155" s="5">
         <v>44979</v>
       </c>
@@ -12544,7 +12514,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="156" spans="1:24">
+    <row r="156" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A156" s="5">
         <v>44979</v>
       </c>
@@ -12608,7 +12578,7 @@
       </c>
       <c r="X156" s="16"/>
     </row>
-    <row r="157" spans="1:24">
+    <row r="157" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A157" s="5">
         <v>44979</v>
       </c>
@@ -12672,7 +12642,7 @@
       </c>
       <c r="X157" s="16"/>
     </row>
-    <row r="158" spans="1:24">
+    <row r="158" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A158" s="7">
         <v>44981</v>
       </c>
@@ -12736,7 +12706,7 @@
       </c>
       <c r="X158" s="16"/>
     </row>
-    <row r="159" spans="1:24">
+    <row r="159" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A159" s="5">
         <v>44987</v>
       </c>
@@ -12800,7 +12770,7 @@
       </c>
       <c r="X159" s="16"/>
     </row>
-    <row r="160" spans="1:24">
+    <row r="160" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A160" s="5">
         <v>44987</v>
       </c>
@@ -12864,7 +12834,7 @@
       </c>
       <c r="X160" s="16"/>
     </row>
-    <row r="161" spans="1:24">
+    <row r="161" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A161" s="7">
         <v>44991</v>
       </c>
@@ -12930,7 +12900,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="162" spans="1:24">
+    <row r="162" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A162" s="7">
         <v>44992</v>
       </c>
@@ -12994,7 +12964,7 @@
       </c>
       <c r="X162" s="16"/>
     </row>
-    <row r="163" spans="1:24">
+    <row r="163" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A163" s="5">
         <v>44993</v>
       </c>
@@ -13010,16 +12980,16 @@
       <c r="E163" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F163" s="48">
+      <c r="F163" s="35">
         <v>541</v>
       </c>
-      <c r="G163" s="48">
+      <c r="G163" s="35">
         <v>9.4</v>
       </c>
-      <c r="H163" s="45">
+      <c r="H163" s="6">
         <v>80.099999999999994</v>
       </c>
-      <c r="I163" s="45">
+      <c r="I163" s="6">
         <v>49.7</v>
       </c>
       <c r="J163" s="1">
@@ -13066,7 +13036,7 @@
       </c>
       <c r="X163" s="16"/>
     </row>
-    <row r="164" spans="1:24">
+    <row r="164" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A164" s="5">
         <v>44993</v>
       </c>
@@ -13082,16 +13052,16 @@
       <c r="E164" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F164" s="48">
+      <c r="F164" s="35">
         <v>541</v>
       </c>
-      <c r="G164" s="48">
+      <c r="G164" s="35">
         <v>9.4</v>
       </c>
-      <c r="H164" s="45">
+      <c r="H164" s="6">
         <v>80.099999999999994</v>
       </c>
-      <c r="I164" s="45">
+      <c r="I164" s="6">
         <v>49.7</v>
       </c>
       <c r="J164" s="1">
@@ -13138,7 +13108,7 @@
       </c>
       <c r="X164" s="16"/>
     </row>
-    <row r="165" spans="1:24">
+    <row r="165" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A165" s="5">
         <v>44998</v>
       </c>
@@ -13154,16 +13124,16 @@
       <c r="E165" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F165" s="48">
+      <c r="F165" s="35">
         <v>127</v>
       </c>
-      <c r="G165" s="48">
+      <c r="G165" s="35">
         <v>9.5</v>
       </c>
-      <c r="H165" s="45">
+      <c r="H165" s="6">
         <v>19.8</v>
       </c>
-      <c r="I165" s="45">
+      <c r="I165" s="6">
         <v>21.2</v>
       </c>
       <c r="J165" s="1">
@@ -13210,7 +13180,7 @@
       </c>
       <c r="X165" s="16"/>
     </row>
-    <row r="166" spans="1:24">
+    <row r="166" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A166" s="5">
         <v>44998</v>
       </c>
@@ -13226,16 +13196,16 @@
       <c r="E166" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="F166" s="48">
+      <c r="F166" s="35">
         <v>209</v>
       </c>
-      <c r="G166" s="48">
+      <c r="G166" s="35">
         <v>10.3</v>
       </c>
-      <c r="H166" s="45">
+      <c r="H166" s="6">
         <v>36</v>
       </c>
-      <c r="I166" s="45">
+      <c r="I166" s="6">
         <v>21.8</v>
       </c>
       <c r="J166" s="1">
@@ -13282,7 +13252,7 @@
       </c>
       <c r="X166" s="16"/>
     </row>
-    <row r="167" spans="1:24">
+    <row r="167" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A167" s="5">
         <v>45000</v>
       </c>
@@ -13298,16 +13268,16 @@
       <c r="E167" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F167" s="48">
+      <c r="F167" s="35">
         <v>928</v>
       </c>
-      <c r="G167" s="48">
+      <c r="G167" s="35">
         <v>10.4</v>
       </c>
-      <c r="H167" s="45">
+      <c r="H167" s="6">
         <v>17.7</v>
       </c>
-      <c r="I167" s="45">
+      <c r="I167" s="6">
         <v>20.399999999999999</v>
       </c>
       <c r="J167" s="1">
@@ -13354,7 +13324,7 @@
       </c>
       <c r="X167" s="16"/>
     </row>
-    <row r="168" spans="1:24">
+    <row r="168" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A168" s="5">
         <v>45000</v>
       </c>
@@ -13370,16 +13340,16 @@
       <c r="E168" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="F168" s="48">
+      <c r="F168" s="35">
         <v>171</v>
       </c>
-      <c r="G168" s="48">
+      <c r="G168" s="35">
         <v>10.6</v>
       </c>
-      <c r="H168" s="45">
+      <c r="H168" s="6">
         <v>43.9</v>
       </c>
-      <c r="I168" s="45">
+      <c r="I168" s="6">
         <v>28</v>
       </c>
       <c r="J168" s="1">
@@ -13426,7 +13396,7 @@
       </c>
       <c r="X168" s="16"/>
     </row>
-    <row r="169" spans="1:24">
+    <row r="169" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A169" s="5">
         <v>45000</v>
       </c>
@@ -13442,16 +13412,16 @@
       <c r="E169" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="F169" s="48">
+      <c r="F169" s="35">
         <v>338</v>
       </c>
-      <c r="G169" s="48">
+      <c r="G169" s="35">
         <v>11.2</v>
       </c>
-      <c r="H169" s="45">
+      <c r="H169" s="6">
         <v>147</v>
       </c>
-      <c r="I169" s="45">
+      <c r="I169" s="6">
         <v>84.2</v>
       </c>
       <c r="J169" s="1">
@@ -13498,7 +13468,7 @@
       </c>
       <c r="X169" s="16"/>
     </row>
-    <row r="170" spans="1:24">
+    <row r="170" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" s="5">
         <v>45000</v>
       </c>
@@ -13514,16 +13484,16 @@
       <c r="E170" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="F170" s="48">
+      <c r="F170" s="35">
         <v>338</v>
       </c>
-      <c r="G170" s="48">
+      <c r="G170" s="35">
         <v>11.2</v>
       </c>
-      <c r="H170" s="45">
+      <c r="H170" s="6">
         <v>147</v>
       </c>
-      <c r="I170" s="45">
+      <c r="I170" s="6">
         <v>84.2</v>
       </c>
       <c r="J170" s="1">
@@ -13570,7 +13540,7 @@
       </c>
       <c r="X170" s="16"/>
     </row>
-    <row r="171" spans="1:24">
+    <row r="171" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A171" s="5">
         <v>45000</v>
       </c>
@@ -13586,16 +13556,16 @@
       <c r="E171" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F171" s="48">
+      <c r="F171" s="35">
         <v>189</v>
       </c>
-      <c r="G171" s="48">
+      <c r="G171" s="35">
         <v>11.6</v>
       </c>
-      <c r="H171" s="45">
+      <c r="H171" s="6">
         <v>39.299999999999997</v>
       </c>
-      <c r="I171" s="45">
+      <c r="I171" s="6">
         <v>32.1</v>
       </c>
       <c r="J171" s="1">
@@ -13642,7 +13612,7 @@
       </c>
       <c r="X171" s="16"/>
     </row>
-    <row r="172" spans="1:24">
+    <row r="172" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A172" s="5">
         <v>45000</v>
       </c>
@@ -13658,16 +13628,16 @@
       <c r="E172" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F172" s="48">
+      <c r="F172" s="35">
         <v>189</v>
       </c>
-      <c r="G172" s="48">
+      <c r="G172" s="35">
         <v>11.6</v>
       </c>
-      <c r="H172" s="45">
+      <c r="H172" s="6">
         <v>39.299999999999997</v>
       </c>
-      <c r="I172" s="45">
+      <c r="I172" s="6">
         <v>32.1</v>
       </c>
       <c r="J172" s="1">
@@ -13714,7 +13684,7 @@
       </c>
       <c r="X172" s="16"/>
     </row>
-    <row r="173" spans="1:24">
+    <row r="173" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A173" s="5">
         <v>45002</v>
       </c>
@@ -13730,16 +13700,16 @@
       <c r="E173" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F173" s="48">
+      <c r="F173" s="35">
         <v>193</v>
       </c>
-      <c r="G173" s="48">
+      <c r="G173" s="35">
         <v>11.2</v>
       </c>
-      <c r="H173" s="45">
+      <c r="H173" s="6">
         <v>29.5</v>
       </c>
-      <c r="I173" s="45">
+      <c r="I173" s="6">
         <v>24.4</v>
       </c>
       <c r="J173" s="1">
@@ -13786,7 +13756,7 @@
       </c>
       <c r="X173" s="16"/>
     </row>
-    <row r="174" spans="1:24">
+    <row r="174" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A174" s="5">
         <v>45002</v>
       </c>
@@ -13802,16 +13772,16 @@
       <c r="E174" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F174" s="48">
+      <c r="F174" s="35">
         <v>193</v>
       </c>
-      <c r="G174" s="48">
+      <c r="G174" s="35">
         <v>11.2</v>
       </c>
-      <c r="H174" s="45">
+      <c r="H174" s="6">
         <v>29.5</v>
       </c>
-      <c r="I174" s="45">
+      <c r="I174" s="6">
         <v>24.4</v>
       </c>
       <c r="J174" s="1">
@@ -13858,7 +13828,7 @@
       </c>
       <c r="X174" s="16"/>
     </row>
-    <row r="175" spans="1:24">
+    <row r="175" spans="1:24" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A175" s="7">
         <v>45006</v>
       </c>
@@ -13922,7 +13892,7 @@
       </c>
       <c r="X175" s="16"/>
     </row>
-    <row r="176" spans="1:24">
+    <row r="176" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A176" s="7">
         <v>45021</v>
       </c>
@@ -13986,7 +13956,7 @@
       </c>
       <c r="X176" s="16"/>
     </row>
-    <row r="177" spans="1:24">
+    <row r="177" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A177" s="7">
         <v>45026</v>
       </c>
@@ -14050,7 +14020,7 @@
       </c>
       <c r="X177" s="16"/>
     </row>
-    <row r="178" spans="1:24">
+    <row r="178" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="5">
         <v>45026</v>
       </c>
@@ -14066,16 +14036,16 @@
       <c r="E178" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F178" s="48">
+      <c r="F178" s="35">
         <v>199</v>
       </c>
-      <c r="G178" s="48">
+      <c r="G178" s="35">
         <v>13.4</v>
       </c>
-      <c r="H178" s="45">
+      <c r="H178" s="6">
         <v>14.4</v>
       </c>
-      <c r="I178" s="45">
+      <c r="I178" s="6">
         <v>15.2</v>
       </c>
       <c r="J178" s="1">
@@ -14122,7 +14092,7 @@
       </c>
       <c r="X178" s="16"/>
     </row>
-    <row r="179" spans="1:24">
+    <row r="179" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="5">
         <v>45027</v>
       </c>
@@ -14138,16 +14108,16 @@
       <c r="E179" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="F179" s="48">
+      <c r="F179" s="35">
         <v>603</v>
       </c>
-      <c r="G179" s="48">
+      <c r="G179" s="35">
         <v>15.1</v>
       </c>
-      <c r="H179" s="45">
+      <c r="H179" s="6">
         <v>31.2</v>
       </c>
-      <c r="I179" s="45">
+      <c r="I179" s="6">
         <v>25</v>
       </c>
       <c r="J179" s="1">
@@ -14194,7 +14164,7 @@
       </c>
       <c r="X179" s="16"/>
     </row>
-    <row r="180" spans="1:24">
+    <row r="180" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="5">
         <v>45027</v>
       </c>
@@ -14210,16 +14180,16 @@
       <c r="E180" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F180" s="48">
+      <c r="F180" s="35">
         <v>146</v>
       </c>
-      <c r="G180" s="48">
+      <c r="G180" s="35">
         <v>13.9</v>
       </c>
-      <c r="H180" s="45">
+      <c r="H180" s="6">
         <v>18.8</v>
       </c>
-      <c r="I180" s="45">
+      <c r="I180" s="6">
         <v>12.3</v>
       </c>
       <c r="J180" s="1">
@@ -14266,7 +14236,7 @@
       </c>
       <c r="X180" s="16"/>
     </row>
-    <row r="181" spans="1:24">
+    <row r="181" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="5">
         <v>45027</v>
       </c>
@@ -14282,16 +14252,16 @@
       <c r="E181" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="F181" s="48">
+      <c r="F181" s="35">
         <v>237</v>
       </c>
-      <c r="G181" s="48">
+      <c r="G181" s="35">
         <v>14.1</v>
       </c>
-      <c r="H181" s="45">
+      <c r="H181" s="6">
         <v>9.6999999999999993</v>
       </c>
-      <c r="I181" s="45">
+      <c r="I181" s="6">
         <v>8.3000000000000007</v>
       </c>
       <c r="J181" s="1">
@@ -14338,7 +14308,7 @@
       </c>
       <c r="X181" s="16"/>
     </row>
-    <row r="182" spans="1:24">
+    <row r="182" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="5">
         <v>45028</v>
       </c>
@@ -14354,16 +14324,16 @@
       <c r="E182" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="F182" s="48">
+      <c r="F182" s="35">
         <v>198</v>
       </c>
-      <c r="G182" s="48">
+      <c r="G182" s="35">
         <v>14.6</v>
       </c>
-      <c r="H182" s="45">
+      <c r="H182" s="6">
         <v>18.600000000000001</v>
       </c>
-      <c r="I182" s="45">
+      <c r="I182" s="6">
         <v>22.8</v>
       </c>
       <c r="J182" s="1">
@@ -14410,7 +14380,7 @@
       </c>
       <c r="X182" s="16"/>
     </row>
-    <row r="183" spans="1:24">
+    <row r="183" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="7">
         <v>45028</v>
       </c>
@@ -14474,7 +14444,7 @@
       </c>
       <c r="X183" s="16"/>
     </row>
-    <row r="184" spans="1:24">
+    <row r="184" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="7">
         <v>45028</v>
       </c>
@@ -14538,7 +14508,7 @@
       </c>
       <c r="X184" s="16"/>
     </row>
-    <row r="185" spans="1:24">
+    <row r="185" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="5">
         <v>45028</v>
       </c>
@@ -14554,16 +14524,16 @@
       <c r="E185" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F185" s="48">
+      <c r="F185" s="35">
         <v>331</v>
       </c>
-      <c r="G185" s="48">
+      <c r="G185" s="35">
         <v>14.7</v>
       </c>
-      <c r="H185" s="45">
+      <c r="H185" s="6">
         <v>22.6</v>
       </c>
-      <c r="I185" s="45">
+      <c r="I185" s="6">
         <v>26.9</v>
       </c>
       <c r="J185" s="1">
@@ -14610,7 +14580,7 @@
       </c>
       <c r="X185" s="16"/>
     </row>
-    <row r="186" spans="1:24">
+    <row r="186" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="5">
         <v>45028</v>
       </c>
@@ -14626,16 +14596,16 @@
       <c r="E186" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F186" s="48">
+      <c r="F186" s="35">
         <v>331</v>
       </c>
-      <c r="G186" s="48">
+      <c r="G186" s="35">
         <v>14.7</v>
       </c>
-      <c r="H186" s="45">
+      <c r="H186" s="6">
         <v>22.6</v>
       </c>
-      <c r="I186" s="45">
+      <c r="I186" s="6">
         <v>26.9</v>
       </c>
       <c r="J186" s="1">
@@ -14682,7 +14652,7 @@
       </c>
       <c r="X186" s="16"/>
     </row>
-    <row r="187" spans="1:24">
+    <row r="187" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A187" s="5">
         <v>45028</v>
       </c>
@@ -14698,16 +14668,16 @@
       <c r="E187" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F187" s="48">
+      <c r="F187" s="35">
         <v>331</v>
       </c>
-      <c r="G187" s="48">
+      <c r="G187" s="35">
         <v>14.7</v>
       </c>
-      <c r="H187" s="45">
+      <c r="H187" s="6">
         <v>22.6</v>
       </c>
-      <c r="I187" s="45">
+      <c r="I187" s="6">
         <v>26.9</v>
       </c>
       <c r="J187" s="1">
@@ -14754,7 +14724,7 @@
       </c>
       <c r="X187" s="16"/>
     </row>
-    <row r="188" spans="1:24">
+    <row r="188" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A188" s="5">
         <v>45028</v>
       </c>
@@ -14770,16 +14740,16 @@
       <c r="E188" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F188" s="48">
+      <c r="F188" s="35">
         <v>331</v>
       </c>
-      <c r="G188" s="48">
+      <c r="G188" s="35">
         <v>14.7</v>
       </c>
-      <c r="H188" s="45">
+      <c r="H188" s="6">
         <v>22.6</v>
       </c>
-      <c r="I188" s="45">
+      <c r="I188" s="6">
         <v>26.9</v>
       </c>
       <c r="J188" s="1">
@@ -14826,7 +14796,7 @@
       </c>
       <c r="X188" s="16"/>
     </row>
-    <row r="189" spans="1:24">
+    <row r="189" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A189" s="5">
         <v>45028</v>
       </c>
@@ -14842,16 +14812,16 @@
       <c r="E189" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="F189" s="48">
+      <c r="F189" s="35">
         <v>331</v>
       </c>
-      <c r="G189" s="48">
+      <c r="G189" s="35">
         <v>14.7</v>
       </c>
-      <c r="H189" s="45">
+      <c r="H189" s="6">
         <v>22.6</v>
       </c>
-      <c r="I189" s="45">
+      <c r="I189" s="6">
         <v>26.9</v>
       </c>
       <c r="J189" s="1">
@@ -14898,7 +14868,7 @@
       </c>
       <c r="X189" s="16"/>
     </row>
-    <row r="190" spans="1:24">
+    <row r="190" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A190" s="7">
         <v>45035</v>
       </c>
@@ -14962,7 +14932,7 @@
       </c>
       <c r="X190" s="16"/>
     </row>
-    <row r="191" spans="1:24">
+    <row r="191" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A191" s="7">
         <v>45036</v>
       </c>
@@ -15026,7 +14996,7 @@
       </c>
       <c r="X191" s="16"/>
     </row>
-    <row r="192" spans="1:24">
+    <row r="192" spans="1:24" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A192" s="5">
         <v>45040</v>
       </c>
@@ -15042,16 +15012,16 @@
       <c r="E192" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F192" s="48">
+      <c r="F192" s="35">
         <v>157</v>
       </c>
-      <c r="G192" s="48">
+      <c r="G192" s="35">
         <v>14.9</v>
       </c>
-      <c r="H192" s="45">
+      <c r="H192" s="6">
         <v>17.600000000000001</v>
       </c>
-      <c r="I192" s="45">
+      <c r="I192" s="6">
         <v>8.9</v>
       </c>
       <c r="J192" s="1">
@@ -15098,7 +15068,7 @@
       </c>
       <c r="X192" s="16"/>
     </row>
-    <row r="193" spans="1:31">
+    <row r="193" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A193" s="5">
         <v>45040</v>
       </c>
@@ -15114,16 +15084,16 @@
       <c r="E193" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="F193" s="48">
+      <c r="F193" s="35">
         <v>155</v>
       </c>
-      <c r="G193" s="48">
+      <c r="G193" s="35">
         <v>16.5</v>
       </c>
-      <c r="H193" s="45">
+      <c r="H193" s="6">
         <v>11.6</v>
       </c>
-      <c r="I193" s="45">
+      <c r="I193" s="6">
         <v>5.4</v>
       </c>
       <c r="J193" s="1">
@@ -15170,7 +15140,7 @@
       </c>
       <c r="X193" s="16"/>
     </row>
-    <row r="194" spans="1:31">
+    <row r="194" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A194" s="7">
         <v>45043</v>
       </c>
@@ -15234,7 +15204,7 @@
       </c>
       <c r="X194" s="16"/>
     </row>
-    <row r="195" spans="1:31">
+    <row r="195" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" s="7">
         <v>45048</v>
       </c>
@@ -15298,7 +15268,7 @@
       </c>
       <c r="X195" s="16"/>
     </row>
-    <row r="196" spans="1:31">
+    <row r="196" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A196" s="7">
         <v>45050</v>
       </c>
@@ -15362,7 +15332,7 @@
       </c>
       <c r="X196" s="16"/>
     </row>
-    <row r="197" spans="1:31">
+    <row r="197" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A197" s="7">
         <v>45054</v>
       </c>
@@ -15426,7 +15396,7 @@
       </c>
       <c r="X197" s="16"/>
     </row>
-    <row r="198" spans="1:31">
+    <row r="198" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A198" s="7">
         <v>45054</v>
       </c>
@@ -15490,7 +15460,7 @@
       </c>
       <c r="X198" s="16"/>
     </row>
-    <row r="199" spans="1:31">
+    <row r="199" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A199" s="7">
         <v>45054</v>
       </c>
@@ -15554,7 +15524,7 @@
       </c>
       <c r="X199" s="16"/>
     </row>
-    <row r="200" spans="1:31">
+    <row r="200" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A200" s="7">
         <v>45070</v>
       </c>
@@ -15618,7 +15588,7 @@
       </c>
       <c r="X200" s="16"/>
     </row>
-    <row r="201" spans="1:31">
+    <row r="201" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A201" s="7">
         <v>45076</v>
       </c>
@@ -15682,7 +15652,7 @@
       </c>
       <c r="X201" s="16"/>
     </row>
-    <row r="202" spans="1:31">
+    <row r="202" spans="1:31" ht="14.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A202" s="7">
         <v>45084</v>
       </c>
@@ -15746,7 +15716,7 @@
       </c>
       <c r="X202" s="16"/>
     </row>
-    <row r="203" spans="1:31" s="14" customFormat="1" ht="15" customHeight="1">
+    <row r="203" spans="1:31" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" s="5">
         <v>45105</v>
       </c>
@@ -15809,7 +15779,7 @@
         <v>14.2</v>
       </c>
     </row>
-    <row r="204" spans="1:31" ht="15" customHeight="1">
+    <row r="204" spans="1:31" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" s="5">
         <v>45114</v>
       </c>
@@ -15873,7 +15843,7 @@
       </c>
       <c r="X204"/>
     </row>
-    <row r="205" spans="1:31" ht="15" customHeight="1">
+    <row r="205" spans="1:31" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" s="22">
         <v>45118</v>
       </c>
@@ -15937,7 +15907,7 @@
       </c>
       <c r="AE205" s="24"/>
     </row>
-    <row r="206" spans="1:31" ht="15" customHeight="1">
+    <row r="206" spans="1:31" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" s="5">
         <v>45159</v>
       </c>
@@ -15953,16 +15923,16 @@
       <c r="E206" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F206" s="48">
+      <c r="F206" s="35">
         <v>3440</v>
       </c>
-      <c r="G206" s="48">
+      <c r="G206" s="35">
         <v>22.8</v>
       </c>
-      <c r="H206" s="45">
+      <c r="H206" s="6">
         <v>27.7</v>
       </c>
-      <c r="I206" s="45"/>
+      <c r="I206" s="6"/>
       <c r="J206" s="1">
         <v>50</v>
       </c>
@@ -16007,7 +15977,7 @@
       </c>
       <c r="X206" s="16"/>
     </row>
-    <row r="207" spans="1:31" s="14" customFormat="1" ht="15" customHeight="1">
+    <row r="207" spans="1:31" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" s="7">
         <v>45190</v>
       </c>
@@ -16070,7 +16040,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="208" spans="1:31" s="14" customFormat="1" ht="15" customHeight="1">
+    <row r="208" spans="1:31" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" s="7">
         <v>45194</v>
       </c>
@@ -16133,73 +16103,73 @@
         <v>72</v>
       </c>
     </row>
-    <row r="209" spans="1:24" s="38" customFormat="1" ht="15" customHeight="1">
-      <c r="A209" s="33">
+    <row r="209" spans="1:24" s="14" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A209" s="7">
         <v>45197</v>
       </c>
-      <c r="B209" s="34" t="s">
+      <c r="B209" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C209" s="35" t="s">
+      <c r="C209" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D209" s="34" t="s">
+      <c r="D209" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="E209" s="34" t="s">
+      <c r="E209" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="F209" s="34"/>
-      <c r="G209" s="34"/>
-      <c r="H209" s="34"/>
-      <c r="I209" s="34"/>
-      <c r="J209" s="34">
+      <c r="F209" s="4"/>
+      <c r="G209" s="4"/>
+      <c r="H209" s="4"/>
+      <c r="I209" s="4"/>
+      <c r="J209" s="4">
         <v>70</v>
       </c>
-      <c r="K209" s="34" t="s">
+      <c r="K209" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="L209" s="34">
+      <c r="L209" s="4">
         <v>38.083379999999998</v>
       </c>
-      <c r="M209" s="34">
+      <c r="M209" s="4">
         <v>-122.05802</v>
       </c>
-      <c r="N209" s="36" t="s">
+      <c r="N209" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="O209" s="34" t="s">
+      <c r="O209" s="4" t="s">
         <v>386</v>
       </c>
-      <c r="P209" s="34" t="s">
+      <c r="P209" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="Q209" s="34" t="s">
+      <c r="Q209" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="R209" s="35" t="s">
+      <c r="R209" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="S209" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="T209" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="U209" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="V209" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="W209" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="X209" s="37" t="s">
+      <c r="S209" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="T209" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="U209" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="V209" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="W209" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="X209" s="23" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="210" spans="1:24" ht="15" customHeight="1">
+    <row r="210" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" s="22">
         <v>45204</v>
       </c>
@@ -16260,7 +16230,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="211" spans="1:24" ht="15" customHeight="1">
+    <row r="211" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A211" s="22">
         <v>45223</v>
       </c>
@@ -16321,7 +16291,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="212" spans="1:24" ht="15" customHeight="1">
+    <row r="212" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" s="22">
         <v>45245</v>
       </c>
@@ -16351,13 +16321,13 @@
       <c r="M212" s="14">
         <v>-121.83794</v>
       </c>
-      <c r="N212" s="39" t="s">
+      <c r="N212" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="O212" s="40" t="s">
+      <c r="O212" s="14" t="s">
         <v>393</v>
       </c>
-      <c r="P212" s="41" t="s">
+      <c r="P212" s="4" t="s">
         <v>86</v>
       </c>
       <c r="Q212" s="4" t="s">
@@ -16382,7 +16352,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="213" spans="1:24" ht="15" customHeight="1">
+    <row r="213" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" s="22">
         <v>45267</v>
       </c>
@@ -16412,13 +16382,13 @@
       <c r="M213" s="14">
         <v>-121.75851</v>
       </c>
-      <c r="N213" s="39" t="s">
+      <c r="N213" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O213" s="40" t="s">
+      <c r="O213" s="14" t="s">
         <v>395</v>
       </c>
-      <c r="P213" s="40" t="s">
+      <c r="P213" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q213" s="14" t="s">
@@ -16439,9 +16409,8 @@
       <c r="V213" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W213" s="38"/>
-    </row>
-    <row r="214" spans="1:24" ht="15" customHeight="1">
+    </row>
+    <row r="214" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" s="22">
         <v>45307</v>
       </c>
@@ -16471,13 +16440,13 @@
       <c r="M214" s="14">
         <v>-121.78878</v>
       </c>
-      <c r="N214" s="39" t="s">
+      <c r="N214" s="8" t="s">
         <v>381</v>
       </c>
-      <c r="O214" s="40" t="s">
+      <c r="O214" s="14" t="s">
         <v>400</v>
       </c>
-      <c r="P214" s="40" t="s">
+      <c r="P214" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q214" s="14" t="s">
@@ -16498,9 +16467,8 @@
       <c r="V214" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W214" s="38"/>
-    </row>
-    <row r="215" spans="1:24" ht="15" customHeight="1">
+    </row>
+    <row r="215" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" s="22">
         <v>45313</v>
       </c>
@@ -16530,13 +16498,13 @@
       <c r="M215" s="14">
         <v>-121.89997</v>
       </c>
-      <c r="N215" s="41" t="s">
+      <c r="N215" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="O215" s="42" t="s">
+      <c r="O215" s="4" t="s">
         <v>405</v>
       </c>
-      <c r="P215" s="41" t="s">
+      <c r="P215" s="4" t="s">
         <v>406</v>
       </c>
       <c r="Q215" s="14" t="s">
@@ -16557,12 +16525,11 @@
       <c r="V215" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W215" s="38"/>
       <c r="X215" s="16" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="216" spans="1:24" ht="15" customHeight="1">
+    <row r="216" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A216" s="22">
         <v>45313</v>
       </c>
@@ -16592,19 +16559,19 @@
       <c r="M216" s="14">
         <v>-122.08213000000001</v>
       </c>
-      <c r="N216" s="41" t="s">
+      <c r="N216" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="O216" s="42" t="s">
+      <c r="O216" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="P216" s="41" t="s">
+      <c r="P216" s="4" t="s">
         <v>75</v>
       </c>
       <c r="Q216" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="R216" s="34" t="s">
+      <c r="R216" s="4" t="s">
         <v>75</v>
       </c>
       <c r="S216" s="4" t="s">
@@ -16626,7 +16593,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="217" spans="1:24" ht="15" customHeight="1">
+    <row r="217" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" s="22">
         <v>45315</v>
       </c>
@@ -16656,13 +16623,13 @@
       <c r="M217" s="14">
         <v>-122.06549</v>
       </c>
-      <c r="N217" s="39" t="s">
+      <c r="N217" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O217" s="42" t="s">
+      <c r="O217" s="4" t="s">
         <v>412</v>
       </c>
-      <c r="P217" s="40" t="s">
+      <c r="P217" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q217" s="14" t="s">
@@ -16683,9 +16650,8 @@
       <c r="V217" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W217" s="38"/>
-    </row>
-    <row r="218" spans="1:24" ht="15" customHeight="1">
+    </row>
+    <row r="218" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" s="22">
         <v>45315</v>
       </c>
@@ -16715,13 +16681,13 @@
       <c r="M218" s="14">
         <v>-121.65279</v>
       </c>
-      <c r="N218" s="39" t="s">
+      <c r="N218" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O218" s="42" t="s">
+      <c r="O218" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="P218" s="40" t="s">
+      <c r="P218" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q218" s="14" t="s">
@@ -16742,9 +16708,8 @@
       <c r="V218" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W218" s="38"/>
-    </row>
-    <row r="219" spans="1:24" ht="15" customHeight="1">
+    </row>
+    <row r="219" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" s="22">
         <v>45316</v>
       </c>
@@ -16774,13 +16739,13 @@
       <c r="M219" s="14">
         <v>-121.7368</v>
       </c>
-      <c r="N219" s="39" t="s">
+      <c r="N219" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O219" s="42" t="s">
+      <c r="O219" s="4" t="s">
         <v>417</v>
       </c>
-      <c r="P219" s="40" t="s">
+      <c r="P219" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q219" s="14" t="s">
@@ -16801,9 +16766,8 @@
       <c r="V219" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="W219" s="38"/>
-    </row>
-    <row r="220" spans="1:24" ht="15" customHeight="1">
+    </row>
+    <row r="220" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" s="22">
         <v>45318</v>
       </c>
@@ -16835,17 +16799,17 @@
       <c r="M220" s="14">
         <v>-121.558995</v>
       </c>
-      <c r="N220" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="O220" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="P220" s="40" t="s">
+      <c r="N220" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O220" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="P220" s="14" t="s">
         <v>118</v>
       </c>
       <c r="Q220" s="14" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="R220" s="14" t="s">
         <v>77</v>
@@ -16862,9 +16826,8 @@
       <c r="V220" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W220" s="38"/>
-    </row>
-    <row r="221" spans="1:24" ht="15" customHeight="1">
+    </row>
+    <row r="221" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" s="22">
         <v>45322</v>
       </c>
@@ -16894,13 +16857,13 @@
       <c r="M221" s="14">
         <v>-121.55394</v>
       </c>
-      <c r="N221" s="39" t="s">
+      <c r="N221" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O221" s="42" t="s">
+      <c r="O221" s="4" t="s">
         <v>422</v>
       </c>
-      <c r="P221" s="40" t="s">
+      <c r="P221" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q221" s="14" t="s">
@@ -16921,9 +16884,8 @@
       <c r="V221" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="W221" s="38"/>
-    </row>
-    <row r="222" spans="1:24" ht="15" customHeight="1">
+    </row>
+    <row r="222" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" s="22">
         <v>45323</v>
       </c>
@@ -16953,13 +16915,13 @@
       <c r="M222" s="14">
         <v>-121.98945000000001</v>
       </c>
-      <c r="N222" s="39" t="s">
+      <c r="N222" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O222" s="42" t="s">
+      <c r="O222" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="P222" s="40" t="s">
+      <c r="P222" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q222" s="14" t="s">
@@ -16980,9 +16942,8 @@
       <c r="V222" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W222" s="38"/>
-    </row>
-    <row r="223" spans="1:24" ht="15" customHeight="1">
+    </row>
+    <row r="223" spans="1:24" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" s="22">
         <v>45327</v>
       </c>
@@ -17000,10 +16961,10 @@
       </c>
       <c r="F223" s="14"/>
       <c r="G223" s="14"/>
-      <c r="J223" s="38" t="s">
+      <c r="J223" s="14" t="s">
         <v>404</v>
       </c>
-      <c r="K223" s="38" t="s">
+      <c r="K223" s="14" t="s">
         <v>73</v>
       </c>
       <c r="L223" s="14">
@@ -17012,13 +16973,13 @@
       <c r="M223" s="14">
         <v>-122.04123</v>
       </c>
-      <c r="N223" s="41" t="s">
+      <c r="N223" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="O223" s="40" t="s">
+      <c r="O223" s="14" t="s">
         <v>426</v>
       </c>
-      <c r="P223" s="40" t="s">
+      <c r="P223" s="14" t="s">
         <v>262</v>
       </c>
       <c r="Q223" s="14" t="s">
@@ -17042,11 +17003,11 @@
       <c r="W223" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="X223" s="44" t="s">
+      <c r="X223" s="33" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="224" spans="1:24" ht="15" customHeight="1">
+    <row r="224" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" s="22">
         <v>45327</v>
       </c>
@@ -17076,13 +17037,13 @@
       <c r="M224" s="14">
         <v>-121.89077</v>
       </c>
-      <c r="N224" s="39" t="s">
+      <c r="N224" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O224" s="40" t="s">
+      <c r="O224" s="14" t="s">
         <v>430</v>
       </c>
-      <c r="P224" s="40" t="s">
+      <c r="P224" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q224" s="14" t="s">
@@ -17103,9 +17064,8 @@
       <c r="V224" s="14" t="s">
         <v>420</v>
       </c>
-      <c r="W224" s="38"/>
-    </row>
-    <row r="225" spans="1:23" ht="15" customHeight="1">
+    </row>
+    <row r="225" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" s="22">
         <v>45327</v>
       </c>
@@ -17135,13 +17095,13 @@
       <c r="M225" s="14">
         <v>-121.75342999999999</v>
       </c>
-      <c r="N225" s="39" t="s">
+      <c r="N225" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O225" s="40" t="s">
+      <c r="O225" s="14" t="s">
         <v>433</v>
       </c>
-      <c r="P225" s="40" t="s">
+      <c r="P225" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q225" s="14" t="s">
@@ -17162,9 +17122,8 @@
       <c r="V225" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W225" s="38"/>
-    </row>
-    <row r="226" spans="1:23" ht="15" customHeight="1">
+    </row>
+    <row r="226" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" s="22">
         <v>45327</v>
       </c>
@@ -17194,13 +17153,13 @@
       <c r="M226" s="14">
         <v>-121.75342999999999</v>
       </c>
-      <c r="N226" s="39" t="s">
+      <c r="N226" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="O226" s="40" t="s">
+      <c r="O226" s="14" t="s">
         <v>434</v>
       </c>
-      <c r="P226" s="40" t="s">
+      <c r="P226" s="14" t="s">
         <v>86</v>
       </c>
       <c r="Q226" s="14" t="s">
@@ -17221,9 +17180,8 @@
       <c r="V226" s="14" t="s">
         <v>437</v>
       </c>
-      <c r="W226" s="38"/>
-    </row>
-    <row r="227" spans="1:23" ht="15" customHeight="1">
+    </row>
+    <row r="227" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" s="22">
         <v>45327</v>
       </c>
@@ -17280,9 +17238,8 @@
       <c r="V227" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W227" s="38"/>
-    </row>
-    <row r="228" spans="1:23" ht="15" customHeight="1">
+    </row>
+    <row r="228" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" s="22">
         <v>45328</v>
       </c>
@@ -17339,9 +17296,8 @@
       <c r="V228" s="14" t="s">
         <v>398</v>
       </c>
-      <c r="W228" s="38"/>
-    </row>
-    <row r="229" spans="1:23" ht="15" customHeight="1">
+    </row>
+    <row r="229" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" s="22">
         <v>45328</v>
       </c>
@@ -17373,17 +17329,17 @@
       <c r="M229" s="14">
         <v>-121.558995</v>
       </c>
-      <c r="N229" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="O229" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="P229" s="40" t="s">
+      <c r="N229" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O229" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="P229" s="14" t="s">
         <v>118</v>
       </c>
       <c r="Q229" s="14" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="R229" s="14" t="s">
         <v>77</v>
@@ -17401,7 +17357,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="230" spans="1:23" ht="15" customHeight="1">
+    <row r="230" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" s="22">
         <v>45328</v>
       </c>
@@ -17433,17 +17389,17 @@
       <c r="M230" s="14">
         <v>-121.558995</v>
       </c>
-      <c r="N230" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="O230" s="43" t="s">
-        <v>72</v>
-      </c>
-      <c r="P230" s="40" t="s">
+      <c r="N230" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O230" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="P230" s="14" t="s">
         <v>118</v>
       </c>
       <c r="Q230" s="14" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="R230" s="14" t="s">
         <v>435</v>
@@ -17461,7 +17417,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="231" spans="1:23" ht="15" customHeight="1">
+    <row r="231" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" s="22">
         <v>45329</v>
       </c>
@@ -17480,9 +17436,17 @@
       <c r="J231" s="14">
         <v>58</v>
       </c>
-      <c r="N231" s="39"/>
-      <c r="O231" s="43"/>
-      <c r="P231" s="40"/>
+      <c r="K231" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L231" s="6">
+        <v>38.067970000000003</v>
+      </c>
+      <c r="M231" s="6">
+        <v>-121.82071999999999</v>
+      </c>
+      <c r="N231" s="8"/>
+      <c r="O231" s="19"/>
       <c r="R231" s="14" t="s">
         <v>435</v>
       </c>
@@ -17499,7 +17463,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="232" spans="1:23" ht="15" customHeight="1">
+    <row r="232" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" s="22">
         <v>45330</v>
       </c>
@@ -17518,9 +17482,17 @@
       <c r="J232" s="14">
         <v>69</v>
       </c>
-      <c r="N232" s="39"/>
-      <c r="O232" s="43"/>
-      <c r="P232" s="40"/>
+      <c r="K232" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L232" s="6">
+        <v>38.11177</v>
+      </c>
+      <c r="M232" s="6">
+        <v>-121.69177000000001</v>
+      </c>
+      <c r="N232" s="8"/>
+      <c r="O232" s="19"/>
       <c r="R232" s="14" t="s">
         <v>441</v>
       </c>
@@ -17537,7 +17509,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="233" spans="1:23" ht="15" customHeight="1">
+    <row r="233" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" s="22">
         <v>45330</v>
       </c>
@@ -17556,9 +17528,17 @@
       <c r="J233" s="14">
         <v>68</v>
       </c>
-      <c r="N233" s="39"/>
-      <c r="O233" s="43"/>
-      <c r="P233" s="40"/>
+      <c r="K233" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L233" s="6">
+        <v>38.074460000000002</v>
+      </c>
+      <c r="M233" s="6">
+        <v>-121.57089999999999</v>
+      </c>
+      <c r="N233" s="8"/>
+      <c r="O233" s="19"/>
       <c r="R233" s="14" t="s">
         <v>435</v>
       </c>
@@ -17575,7 +17555,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="234" spans="1:23" ht="15" customHeight="1">
+    <row r="234" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A234" s="22">
         <v>45331</v>
       </c>
@@ -17605,11 +17585,11 @@
       <c r="M234" s="14">
         <v>-121.558995</v>
       </c>
-      <c r="N234" s="39" t="s">
+      <c r="N234" s="8" t="s">
         <v>72</v>
       </c>
       <c r="Q234" s="14" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="R234" s="14" t="s">
         <v>444</v>
@@ -17627,7 +17607,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="235" spans="1:23" ht="15" customHeight="1">
+    <row r="235" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A235" s="22">
         <v>45332</v>
       </c>
@@ -17655,11 +17635,11 @@
       <c r="M235" s="14">
         <v>-121.558995</v>
       </c>
-      <c r="N235" s="39" t="s">
+      <c r="N235" s="8" t="s">
         <v>72</v>
       </c>
       <c r="Q235" s="14" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="R235" s="14" t="s">
         <v>77</v>
@@ -17677,7 +17657,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="236" spans="1:23" ht="15" customHeight="1">
+    <row r="236" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A236" s="22">
         <v>45334</v>
       </c>
@@ -17705,11 +17685,11 @@
       <c r="M236" s="14">
         <v>-121.558995</v>
       </c>
-      <c r="N236" s="39" t="s">
+      <c r="N236" s="8" t="s">
         <v>72</v>
       </c>
       <c r="Q236" s="14" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="R236" s="14" t="s">
         <v>441</v>
@@ -17727,20 +17707,31 @@
         <v>443</v>
       </c>
     </row>
-    <row r="237" spans="1:23" ht="15" customHeight="1">
+    <row r="237" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" s="22">
         <v>45334</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="C237" s="1"/>
+      <c r="C237" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="D237" s="1"/>
       <c r="E237" s="1"/>
       <c r="J237" s="14">
         <v>70</v>
       </c>
-      <c r="N237" s="39"/>
+      <c r="K237" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L237" s="6">
+        <v>38.047800000000002</v>
+      </c>
+      <c r="M237" s="6">
+        <v>-122.1733</v>
+      </c>
+      <c r="N237" s="8"/>
       <c r="R237" s="14" t="s">
         <v>418</v>
       </c>
@@ -17757,7 +17748,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="238" spans="1:23" ht="15" customHeight="1">
+    <row r="238" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A238" s="22">
         <v>45335</v>
       </c>
@@ -17785,11 +17776,11 @@
       <c r="M238" s="14">
         <v>-121.558995</v>
       </c>
-      <c r="N238" s="39" t="s">
+      <c r="N238" s="8" t="s">
         <v>72</v>
       </c>
       <c r="Q238" s="14" t="s">
-        <v>336</v>
+        <v>128</v>
       </c>
       <c r="R238" s="14" t="s">
         <v>441</v>
@@ -17807,8 +17798,201 @@
         <v>443</v>
       </c>
     </row>
+    <row r="239" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A239" s="22">
+        <v>45335</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="C239" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D239" s="1"/>
+      <c r="E239" s="1"/>
+      <c r="J239" s="14">
+        <v>78</v>
+      </c>
+      <c r="K239" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L239" s="6">
+        <v>38.094329999999999</v>
+      </c>
+      <c r="M239" s="6">
+        <v>-121.59090999999999</v>
+      </c>
+      <c r="N239" s="8"/>
+      <c r="R239" s="14" t="s">
+        <v>435</v>
+      </c>
+      <c r="S239" s="14" t="s">
+        <v>436</v>
+      </c>
+      <c r="T239" s="22">
+        <v>45316</v>
+      </c>
+      <c r="U239" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="V239" s="14" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="240" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A240" s="22">
+        <v>45335</v>
+      </c>
+      <c r="B240" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C240" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="D240" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E240" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="J240" s="14">
+        <v>84</v>
+      </c>
+      <c r="K240" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L240" s="14">
+        <v>37.815818999999998</v>
+      </c>
+      <c r="M240" s="14">
+        <v>-121.558995</v>
+      </c>
+      <c r="N240" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q240" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="R240" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="S240" s="14" t="s">
+        <v>401</v>
+      </c>
+      <c r="T240" s="22">
+        <v>45301</v>
+      </c>
+      <c r="U240" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="V240" s="14" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="241" spans="1:22" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A241" s="22">
+        <v>45336</v>
+      </c>
+      <c r="B241" s="14" t="s">
+        <v>446</v>
+      </c>
+      <c r="C241" s="14" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="242" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A242" s="22">
+        <v>45336</v>
+      </c>
+      <c r="B242" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="C242" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J242" s="14">
+        <v>61</v>
+      </c>
+      <c r="K242" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L242" s="6">
+        <v>38.186019999999999</v>
+      </c>
+      <c r="M242" s="6">
+        <v>-121.98199</v>
+      </c>
+      <c r="R242" s="14" t="s">
+        <v>441</v>
+      </c>
+      <c r="S242" s="14" t="s">
+        <v>442</v>
+      </c>
+      <c r="T242" s="22">
+        <v>45322</v>
+      </c>
+      <c r="U242" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="V242" s="14" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="243" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A243" s="22">
+        <v>45336</v>
+      </c>
+      <c r="B243" s="14" t="s">
+        <v>402</v>
+      </c>
+      <c r="C243" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J243" s="14">
+        <v>63</v>
+      </c>
+      <c r="K243" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L243" s="6">
+        <v>38.0715</v>
+      </c>
+      <c r="M243" s="6">
+        <v>-121.87093</v>
+      </c>
+      <c r="R243" s="14" t="s">
+        <v>444</v>
+      </c>
+      <c r="S243" s="14" t="s">
+        <v>445</v>
+      </c>
+      <c r="T243" s="22">
+        <v>45321</v>
+      </c>
+      <c r="U243" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="V243" s="14" t="s">
+        <v>437</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:X234" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
+  <autoFilter ref="A1:X243" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
+    <filterColumn colId="17">
+      <filters>
+        <filter val="AdClipped"/>
+        <filter val="VIE-Left/Green/Anterior Dorsal"/>
+        <filter val="VIE-Left/Orange/Anterior Dorsal"/>
+        <filter val="VIE-Left/Orange/Posterior Dorsal"/>
+        <filter val="VIE-Left/Red/Anterior Dorsal"/>
+        <filter val="VIE-Left/Red/Posterior Dorsal"/>
+        <filter val="VIE-Right/Green/Posterior Dorsal"/>
+        <filter val="VIE-Right/Orange/Anterior Dorsal"/>
+        <filter val="VIE-Right/Orange/Posterior Dorsal"/>
+        <filter val="VIE-Right/Red/Anterior Dorsal"/>
+        <filter val="VIE-Right/Red/Mid-dorsal"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X216">
       <sortCondition ref="A1:A213"/>
     </sortState>
@@ -18058,15 +18242,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
@@ -18077,14 +18252,49 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76D96E8C-3FF7-4769-9DB8-E43AB53278F6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76D96E8C-3FF7-4769-9DB8-E43AB53278F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
+    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4F8AF6-B64B-4962-81B5-D73EE7A1E0CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
+    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4F8AF6-B64B-4962-81B5-D73EE7A1E0CA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update smelt catch 2/23 and minor ajustments to plots
</commit_message>
<xml_diff>
--- a/Running Delta Smelt Catch_2023-09-05.xlsx
+++ b/Running Delta Smelt Catch_2023-09-05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/SmeltMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="6_{D7D8C1E3-0910-435B-88BC-04AB77536274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90018AFA-48F1-4A9E-830D-4B830CAD046C}"/>
+  <xr:revisionPtr revIDLastSave="71" documentId="6_{D7D8C1E3-0910-435B-88BC-04AB77536274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA0E7E48-9440-47D9-BFA8-9DD29DF09255}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
+    <workbookView xWindow="28800" yWindow="300" windowWidth="28950" windowHeight="16215" firstSheet="1" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="12" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3485" uniqueCount="451">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="452">
   <si>
     <t>Running Delta Smelt Catch Data Collected for the USFWS Delta Smelt Experimental Release Technical Team</t>
   </si>
@@ -1413,6 +1413,9 @@
   </si>
   <si>
     <t>Water temp channel 10.9, water temp shore 11.0</t>
+  </si>
+  <si>
+    <t>Not included in salvage count, observed in secondary traveling screen</t>
   </si>
 </sst>
 </file>
@@ -2349,10 +2352,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
-  <dimension ref="A1:AE243"/>
+  <dimension ref="A1:AE248"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="E160" sqref="E160"/>
+    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
+      <selection activeCell="K252" sqref="K252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -18080,6 +18083,313 @@
       <c r="AD243" s="41"/>
       <c r="AE243" s="41"/>
     </row>
+    <row r="244" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A244" s="37">
+        <v>45339</v>
+      </c>
+      <c r="B244" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C244" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D244" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E244" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F244" s="39"/>
+      <c r="G244" s="39"/>
+      <c r="H244" s="38"/>
+      <c r="I244" s="38"/>
+      <c r="J244" s="38">
+        <v>58</v>
+      </c>
+      <c r="K244" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L244" s="38">
+        <v>37.815818999999998</v>
+      </c>
+      <c r="M244" s="38">
+        <v>-121.558995</v>
+      </c>
+      <c r="N244" s="38"/>
+      <c r="O244" s="38"/>
+      <c r="P244" s="38"/>
+      <c r="Q244" s="38"/>
+      <c r="R244" s="38" t="s">
+        <v>441</v>
+      </c>
+      <c r="S244" s="38" t="s">
+        <v>442</v>
+      </c>
+      <c r="T244" s="37">
+        <v>45322</v>
+      </c>
+      <c r="U244" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="V244" s="38" t="s">
+        <v>443</v>
+      </c>
+      <c r="W244" s="38"/>
+      <c r="X244" s="42"/>
+      <c r="Y244" s="41"/>
+      <c r="Z244" s="41"/>
+      <c r="AA244" s="41"/>
+      <c r="AB244" s="41"/>
+      <c r="AC244" s="41"/>
+      <c r="AD244" s="41"/>
+      <c r="AE244" s="41"/>
+    </row>
+    <row r="245" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A245" s="37">
+        <v>45339</v>
+      </c>
+      <c r="B245" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C245" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D245" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E245" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F245" s="39"/>
+      <c r="G245" s="39"/>
+      <c r="H245" s="38"/>
+      <c r="I245" s="38"/>
+      <c r="J245" s="38">
+        <v>69</v>
+      </c>
+      <c r="K245" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L245" s="38">
+        <v>37.815818999999998</v>
+      </c>
+      <c r="M245" s="38">
+        <v>-121.558995</v>
+      </c>
+      <c r="N245" s="38"/>
+      <c r="O245" s="38"/>
+      <c r="P245" s="38"/>
+      <c r="Q245" s="38"/>
+      <c r="R245" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="S245" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="T245" s="37">
+        <v>45301</v>
+      </c>
+      <c r="U245" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="V245" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="W245" s="38"/>
+      <c r="X245" s="42" t="s">
+        <v>451</v>
+      </c>
+      <c r="Y245" s="41"/>
+      <c r="Z245" s="41"/>
+      <c r="AA245" s="41"/>
+      <c r="AB245" s="41"/>
+      <c r="AC245" s="41"/>
+      <c r="AD245" s="41"/>
+      <c r="AE245" s="41"/>
+    </row>
+    <row r="246" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A246" s="37">
+        <v>45340</v>
+      </c>
+      <c r="B246" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C246" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D246" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E246" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F246" s="39"/>
+      <c r="G246" s="39"/>
+      <c r="H246" s="38"/>
+      <c r="I246" s="38"/>
+      <c r="J246" s="38">
+        <v>83</v>
+      </c>
+      <c r="K246" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L246" s="38">
+        <v>37.815818999999998</v>
+      </c>
+      <c r="M246" s="38">
+        <v>-121.558995</v>
+      </c>
+      <c r="N246" s="38"/>
+      <c r="O246" s="38"/>
+      <c r="P246" s="38"/>
+      <c r="Q246" s="38"/>
+      <c r="R246" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="S246" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="T246" s="37">
+        <v>45301</v>
+      </c>
+      <c r="U246" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="V246" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="W246" s="38"/>
+      <c r="X246" s="42"/>
+      <c r="Y246" s="41"/>
+      <c r="Z246" s="41"/>
+      <c r="AA246" s="41"/>
+      <c r="AB246" s="41"/>
+      <c r="AC246" s="41"/>
+      <c r="AD246" s="41"/>
+      <c r="AE246" s="41"/>
+    </row>
+    <row r="247" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A247" s="37">
+        <v>45340</v>
+      </c>
+      <c r="B247" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C247" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D247" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E247" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F247" s="39"/>
+      <c r="G247" s="39"/>
+      <c r="H247" s="38"/>
+      <c r="I247" s="38"/>
+      <c r="J247" s="38">
+        <v>68</v>
+      </c>
+      <c r="K247" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L247" s="38">
+        <v>37.815818999999998</v>
+      </c>
+      <c r="M247" s="38">
+        <v>-121.558995</v>
+      </c>
+      <c r="N247" s="38"/>
+      <c r="O247" s="38"/>
+      <c r="P247" s="38"/>
+      <c r="Q247" s="38"/>
+      <c r="R247" s="38" t="s">
+        <v>441</v>
+      </c>
+      <c r="S247" s="38" t="s">
+        <v>442</v>
+      </c>
+      <c r="T247" s="37">
+        <v>45322</v>
+      </c>
+      <c r="U247" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="V247" s="38" t="s">
+        <v>443</v>
+      </c>
+      <c r="W247" s="38"/>
+      <c r="X247" s="42"/>
+      <c r="Y247" s="41"/>
+      <c r="Z247" s="41"/>
+      <c r="AA247" s="41"/>
+      <c r="AB247" s="41"/>
+      <c r="AC247" s="41"/>
+      <c r="AD247" s="41"/>
+      <c r="AE247" s="41"/>
+    </row>
+    <row r="248" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A248" s="37">
+        <v>45344</v>
+      </c>
+      <c r="B248" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C248" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="D248" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E248" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="F248" s="39"/>
+      <c r="G248" s="39"/>
+      <c r="H248" s="38"/>
+      <c r="I248" s="38"/>
+      <c r="J248" s="38">
+        <v>69</v>
+      </c>
+      <c r="K248" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L248" s="38">
+        <v>37.815818999999998</v>
+      </c>
+      <c r="M248" s="38">
+        <v>-121.558995</v>
+      </c>
+      <c r="N248" s="38"/>
+      <c r="O248" s="38"/>
+      <c r="P248" s="38"/>
+      <c r="Q248" s="38"/>
+      <c r="R248" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="S248" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="T248" s="37">
+        <v>45301</v>
+      </c>
+      <c r="U248" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="V248" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="W248" s="38"/>
+      <c r="X248" s="42"/>
+      <c r="Y248" s="41"/>
+      <c r="Z248" s="41"/>
+      <c r="AA248" s="41"/>
+      <c r="AB248" s="41"/>
+      <c r="AC248" s="41"/>
+      <c r="AD248" s="41"/>
+      <c r="AE248" s="41"/>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X204">
     <sortCondition ref="A2:A204"/>
@@ -18091,26 +18401,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D9A9DE233A30CB4EAECD318FD55378CC" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8fd2cacec9171f93eb894d0689f08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65146633-a755-433a-aacb-5024b6511b89" xmlns:ns3="d8e23be6-d007-4c2c-9265-7d9405abf22e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a569083f6831735b7a488ac820eb0384" ns2:_="" ns3:_="">
     <xsd:import namespace="65146633-a755-433a-aacb-5024b6511b89"/>
@@ -18345,10 +18635,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76D96E8C-3FF7-4769-9DB8-E43AB53278F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
+    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18365,20 +18686,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76D96E8C-3FF7-4769-9DB8-E43AB53278F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
-    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updates 2/26 and tweaking some of the colors. Some still dont' work.
</commit_message>
<xml_diff>
--- a/Running Delta Smelt Catch_2023-09-05.xlsx
+++ b/Running Delta Smelt Catch_2023-09-05.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/SmeltMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="6_{D7D8C1E3-0910-435B-88BC-04AB77536274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BA0E7E48-9440-47D9-BFA8-9DD29DF09255}"/>
+  <xr:revisionPtr revIDLastSave="82" documentId="6_{D7D8C1E3-0910-435B-88BC-04AB77536274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE598C17-ED41-4548-8D22-803A11102F59}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="300" windowWidth="28950" windowHeight="16215" firstSheet="1" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="19180" windowHeight="11400" firstSheet="1" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="12" r:id="rId1"/>
     <sheet name="Delta Smelt Catch Data" sheetId="9" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Delta Smelt Catch Data'!$A$1:$X$234</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Delta Smelt Catch Data'!$A$1:$X$250</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3531" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3547" uniqueCount="451">
   <si>
     <t>Running Delta Smelt Catch Data Collected for the USFWS Delta Smelt Experimental Release Technical Team</t>
   </si>
@@ -1266,9 +1266,6 @@
   </si>
   <si>
     <t>BY2023 LS2</t>
-  </si>
-  <si>
-    <t>EDSM</t>
   </si>
   <si>
     <t>24-26-SM01</t>
@@ -2352,10 +2349,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
-  <dimension ref="A1:AE248"/>
+  <dimension ref="A1:AE250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" workbookViewId="0">
-      <selection activeCell="K252" sqref="K252"/>
+    <sheetView tabSelected="1" topLeftCell="F236" workbookViewId="0">
+      <selection activeCell="L253" sqref="L253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -16512,13 +16509,13 @@
         <v>45313</v>
       </c>
       <c r="B215" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C215" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D215" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E215" s="14" t="s">
         <v>133</v>
@@ -16526,7 +16523,7 @@
       <c r="F215" s="14"/>
       <c r="G215" s="14"/>
       <c r="J215" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K215" s="14" t="s">
         <v>73</v>
@@ -16541,10 +16538,10 @@
         <v>260</v>
       </c>
       <c r="O215" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="P215" s="4" t="s">
         <v>405</v>
-      </c>
-      <c r="P215" s="4" t="s">
-        <v>406</v>
       </c>
       <c r="Q215" s="14" t="s">
         <v>87</v>
@@ -16565,7 +16562,7 @@
         <v>398</v>
       </c>
       <c r="X215" s="16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="216" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -16573,13 +16570,13 @@
         <v>45313</v>
       </c>
       <c r="B216" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C216" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D216" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E216" s="14" t="s">
         <v>133</v>
@@ -16587,7 +16584,7 @@
       <c r="F216" s="14"/>
       <c r="G216" s="14"/>
       <c r="J216" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K216" s="14" t="s">
         <v>73</v>
@@ -16602,7 +16599,7 @@
         <v>74</v>
       </c>
       <c r="O216" s="4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="P216" s="4" t="s">
         <v>75</v>
@@ -16629,7 +16626,7 @@
         <v>72</v>
       </c>
       <c r="X216" s="16" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="217" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -16637,13 +16634,13 @@
         <v>45315</v>
       </c>
       <c r="B217" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C217" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D217" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E217" s="14" t="s">
         <v>133</v>
@@ -16666,7 +16663,7 @@
         <v>84</v>
       </c>
       <c r="O217" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="P217" s="14" t="s">
         <v>86</v>
@@ -16695,16 +16692,16 @@
         <v>45315</v>
       </c>
       <c r="B218" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C218" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D218" s="14" t="s">
+        <v>412</v>
+      </c>
+      <c r="E218" s="14" t="s">
         <v>413</v>
-      </c>
-      <c r="E218" s="14" t="s">
-        <v>414</v>
       </c>
       <c r="F218" s="14"/>
       <c r="G218" s="14"/>
@@ -16724,7 +16721,7 @@
         <v>84</v>
       </c>
       <c r="O218" s="4" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="P218" s="14" t="s">
         <v>86</v>
@@ -16753,13 +16750,13 @@
         <v>45316</v>
       </c>
       <c r="B219" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C219" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D219" s="14" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E219" s="14" t="s">
         <v>71</v>
@@ -16782,7 +16779,7 @@
         <v>84</v>
       </c>
       <c r="O219" s="4" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P219" s="14" t="s">
         <v>86</v>
@@ -16791,10 +16788,10 @@
         <v>87</v>
       </c>
       <c r="R219" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="S219" s="14" t="s">
         <v>418</v>
-      </c>
-      <c r="S219" s="14" t="s">
-        <v>419</v>
       </c>
       <c r="T219" s="22">
         <v>45315</v>
@@ -16803,7 +16800,7 @@
         <v>80</v>
       </c>
       <c r="V219" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="220" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -16871,13 +16868,13 @@
         <v>45322</v>
       </c>
       <c r="B221" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C221" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D221" s="14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E221" s="14" t="s">
         <v>104</v>
@@ -16900,7 +16897,7 @@
         <v>84</v>
       </c>
       <c r="O221" s="4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="P221" s="14" t="s">
         <v>86</v>
@@ -16909,10 +16906,10 @@
         <v>87</v>
       </c>
       <c r="R221" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="S221" s="14" t="s">
         <v>418</v>
-      </c>
-      <c r="S221" s="14" t="s">
-        <v>419</v>
       </c>
       <c r="T221" s="22">
         <v>45315</v>
@@ -16921,7 +16918,7 @@
         <v>80</v>
       </c>
       <c r="V221" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="222" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -16929,13 +16926,13 @@
         <v>45323</v>
       </c>
       <c r="B222" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C222" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D222" s="14" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E222" s="14" t="s">
         <v>133</v>
@@ -16958,7 +16955,7 @@
         <v>84</v>
       </c>
       <c r="O222" s="4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="P222" s="14" t="s">
         <v>86</v>
@@ -16987,13 +16984,13 @@
         <v>45327</v>
       </c>
       <c r="B223" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C223" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D223" s="14" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E223" s="14" t="s">
         <v>133</v>
@@ -17001,7 +16998,7 @@
       <c r="F223" s="14"/>
       <c r="G223" s="14"/>
       <c r="J223" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K223" s="14" t="s">
         <v>73</v>
@@ -17016,13 +17013,13 @@
         <v>260</v>
       </c>
       <c r="O223" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="P223" s="14" t="s">
         <v>262</v>
       </c>
       <c r="Q223" s="14" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="R223" s="14" t="s">
         <v>75</v>
@@ -17043,7 +17040,7 @@
         <v>72</v>
       </c>
       <c r="X223" s="33" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="224" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -17051,13 +17048,13 @@
         <v>45327</v>
       </c>
       <c r="B224" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C224" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D224" s="14" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E224" s="14" t="s">
         <v>133</v>
@@ -17080,7 +17077,7 @@
         <v>84</v>
       </c>
       <c r="O224" s="14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="P224" s="14" t="s">
         <v>86</v>
@@ -17089,10 +17086,10 @@
         <v>87</v>
       </c>
       <c r="R224" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="S224" s="14" t="s">
         <v>418</v>
-      </c>
-      <c r="S224" s="14" t="s">
-        <v>419</v>
       </c>
       <c r="T224" s="22">
         <v>45315</v>
@@ -17101,7 +17098,7 @@
         <v>80</v>
       </c>
       <c r="V224" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="225" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -17109,16 +17106,16 @@
         <v>45327</v>
       </c>
       <c r="B225" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C225" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D225" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="E225" s="14" t="s">
         <v>431</v>
-      </c>
-      <c r="E225" s="14" t="s">
-        <v>432</v>
       </c>
       <c r="F225" s="14"/>
       <c r="G225" s="14"/>
@@ -17138,7 +17135,7 @@
         <v>84</v>
       </c>
       <c r="O225" s="14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="P225" s="14" t="s">
         <v>86</v>
@@ -17167,16 +17164,16 @@
         <v>45327</v>
       </c>
       <c r="B226" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C226" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D226" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="E226" s="14" t="s">
         <v>431</v>
-      </c>
-      <c r="E226" s="14" t="s">
-        <v>432</v>
       </c>
       <c r="F226" s="14"/>
       <c r="G226" s="14"/>
@@ -17196,7 +17193,7 @@
         <v>84</v>
       </c>
       <c r="O226" s="14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="P226" s="14" t="s">
         <v>86</v>
@@ -17205,10 +17202,10 @@
         <v>87</v>
       </c>
       <c r="R226" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="S226" s="14" t="s">
         <v>435</v>
-      </c>
-      <c r="S226" s="14" t="s">
-        <v>436</v>
       </c>
       <c r="T226" s="22">
         <v>45316</v>
@@ -17217,7 +17214,7 @@
         <v>80</v>
       </c>
       <c r="V226" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="227" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -17225,16 +17222,16 @@
         <v>45327</v>
       </c>
       <c r="B227" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C227" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D227" s="14" t="s">
+        <v>430</v>
+      </c>
+      <c r="E227" s="14" t="s">
         <v>431</v>
-      </c>
-      <c r="E227" s="14" t="s">
-        <v>432</v>
       </c>
       <c r="F227" s="14"/>
       <c r="G227" s="14"/>
@@ -17254,7 +17251,7 @@
         <v>84</v>
       </c>
       <c r="O227" s="14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="P227" s="14" t="s">
         <v>86</v>
@@ -17283,13 +17280,13 @@
         <v>45328</v>
       </c>
       <c r="B228" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C228" s="14" t="s">
         <v>69</v>
       </c>
       <c r="D228" s="14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E228" s="14" t="s">
         <v>133</v>
@@ -17312,7 +17309,7 @@
         <v>84</v>
       </c>
       <c r="O228" s="14" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="P228" s="14" t="s">
         <v>86</v>
@@ -17441,10 +17438,10 @@
         <v>128</v>
       </c>
       <c r="R230" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="S230" s="14" t="s">
         <v>435</v>
-      </c>
-      <c r="S230" s="14" t="s">
-        <v>436</v>
       </c>
       <c r="T230" s="22">
         <v>45316</v>
@@ -17453,15 +17450,15 @@
         <v>80</v>
       </c>
       <c r="V230" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="231" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" s="22">
         <v>45329</v>
       </c>
-      <c r="B231" s="1" t="s">
-        <v>402</v>
+      <c r="B231" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="C231" s="1" t="s">
         <v>69</v>
@@ -17487,10 +17484,10 @@
       <c r="N231" s="8"/>
       <c r="O231" s="19"/>
       <c r="R231" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="S231" s="14" t="s">
         <v>435</v>
-      </c>
-      <c r="S231" s="14" t="s">
-        <v>436</v>
       </c>
       <c r="T231" s="22">
         <v>45316</v>
@@ -17499,15 +17496,15 @@
         <v>80</v>
       </c>
       <c r="V231" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="232" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" s="22">
         <v>45330</v>
       </c>
-      <c r="B232" s="1" t="s">
-        <v>402</v>
+      <c r="B232" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="C232" s="1" t="s">
         <v>69</v>
@@ -17533,10 +17530,10 @@
       <c r="N232" s="8"/>
       <c r="O232" s="19"/>
       <c r="R232" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="S232" s="14" t="s">
         <v>441</v>
-      </c>
-      <c r="S232" s="14" t="s">
-        <v>442</v>
       </c>
       <c r="T232" s="22">
         <v>45322</v>
@@ -17545,15 +17542,15 @@
         <v>80</v>
       </c>
       <c r="V232" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="233" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A233" s="22">
         <v>45330</v>
       </c>
-      <c r="B233" s="1" t="s">
-        <v>402</v>
+      <c r="B233" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="C233" s="1" t="s">
         <v>69</v>
@@ -17579,10 +17576,10 @@
       <c r="N233" s="8"/>
       <c r="O233" s="19"/>
       <c r="R233" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="S233" s="14" t="s">
         <v>435</v>
-      </c>
-      <c r="S233" s="14" t="s">
-        <v>436</v>
       </c>
       <c r="T233" s="22">
         <v>45316</v>
@@ -17591,7 +17588,7 @@
         <v>80</v>
       </c>
       <c r="V233" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="234" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -17631,10 +17628,10 @@
         <v>128</v>
       </c>
       <c r="R234" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="S234" s="14" t="s">
         <v>444</v>
-      </c>
-      <c r="S234" s="14" t="s">
-        <v>445</v>
       </c>
       <c r="T234" s="22">
         <v>45321</v>
@@ -17643,7 +17640,7 @@
         <v>80</v>
       </c>
       <c r="V234" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="235" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -17731,10 +17728,10 @@
         <v>128</v>
       </c>
       <c r="R236" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="S236" s="14" t="s">
         <v>441</v>
-      </c>
-      <c r="S236" s="14" t="s">
-        <v>442</v>
       </c>
       <c r="T236" s="22">
         <v>45322</v>
@@ -17743,15 +17740,15 @@
         <v>80</v>
       </c>
       <c r="V236" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="237" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A237" s="22">
         <v>45334</v>
       </c>
-      <c r="B237" s="1" t="s">
-        <v>402</v>
+      <c r="B237" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="C237" s="1" t="s">
         <v>69</v>
@@ -17772,10 +17769,10 @@
       </c>
       <c r="N237" s="8"/>
       <c r="R237" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="S237" s="14" t="s">
         <v>418</v>
-      </c>
-      <c r="S237" s="14" t="s">
-        <v>419</v>
       </c>
       <c r="T237" s="22">
         <v>45315</v>
@@ -17784,7 +17781,7 @@
         <v>80</v>
       </c>
       <c r="V237" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="238" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -17822,10 +17819,10 @@
         <v>128</v>
       </c>
       <c r="R238" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="S238" s="14" t="s">
         <v>441</v>
-      </c>
-      <c r="S238" s="14" t="s">
-        <v>442</v>
       </c>
       <c r="T238" s="22">
         <v>45322</v>
@@ -17834,15 +17831,15 @@
         <v>80</v>
       </c>
       <c r="V238" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="239" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A239" s="22">
         <v>45335</v>
       </c>
-      <c r="B239" s="1" t="s">
-        <v>402</v>
+      <c r="B239" s="14" t="s">
+        <v>68</v>
       </c>
       <c r="C239" s="1" t="s">
         <v>69</v>
@@ -17863,10 +17860,10 @@
       </c>
       <c r="N239" s="8"/>
       <c r="R239" s="14" t="s">
+        <v>434</v>
+      </c>
+      <c r="S239" s="14" t="s">
         <v>435</v>
-      </c>
-      <c r="S239" s="14" t="s">
-        <v>436</v>
       </c>
       <c r="T239" s="22">
         <v>45316</v>
@@ -17875,7 +17872,7 @@
         <v>80</v>
       </c>
       <c r="V239" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="240" spans="1:22" ht="19" customHeight="1" x14ac:dyDescent="0.35">
@@ -17933,7 +17930,7 @@
         <v>45336</v>
       </c>
       <c r="B241" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C241" s="1" t="s">
         <v>69</v>
@@ -17951,10 +17948,10 @@
         <v>-121.98199</v>
       </c>
       <c r="R241" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="S241" s="14" t="s">
         <v>441</v>
-      </c>
-      <c r="S241" s="14" t="s">
-        <v>442</v>
       </c>
       <c r="T241" s="22">
         <v>45322</v>
@@ -17963,7 +17960,7 @@
         <v>80</v>
       </c>
       <c r="V241" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="242" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -17971,7 +17968,7 @@
         <v>45336</v>
       </c>
       <c r="B242" s="14" t="s">
-        <v>402</v>
+        <v>68</v>
       </c>
       <c r="C242" s="1" t="s">
         <v>69</v>
@@ -17989,10 +17986,10 @@
         <v>-121.87093</v>
       </c>
       <c r="R242" s="14" t="s">
+        <v>443</v>
+      </c>
+      <c r="S242" s="14" t="s">
         <v>444</v>
-      </c>
-      <c r="S242" s="14" t="s">
-        <v>445</v>
       </c>
       <c r="T242" s="22">
         <v>45321</v>
@@ -18001,7 +17998,7 @@
         <v>80</v>
       </c>
       <c r="V242" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="243" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -18009,13 +18006,13 @@
         <v>45336</v>
       </c>
       <c r="B243" s="38" t="s">
+        <v>445</v>
+      </c>
+      <c r="C243" s="38" t="s">
         <v>446</v>
       </c>
-      <c r="C243" s="38" t="s">
+      <c r="D243" s="38" t="s">
         <v>447</v>
-      </c>
-      <c r="D243" s="38" t="s">
-        <v>448</v>
       </c>
       <c r="E243" s="38" t="s">
         <v>205</v>
@@ -18048,7 +18045,7 @@
         <v>84</v>
       </c>
       <c r="O243" s="38" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="P243" s="38" t="s">
         <v>86</v>
@@ -18057,10 +18054,10 @@
         <v>87</v>
       </c>
       <c r="R243" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="S243" s="38" t="s">
         <v>441</v>
-      </c>
-      <c r="S243" s="38" t="s">
-        <v>442</v>
       </c>
       <c r="T243" s="37">
         <v>45322</v>
@@ -18069,11 +18066,11 @@
         <v>80</v>
       </c>
       <c r="V243" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="W243" s="38"/>
       <c r="X243" s="42" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="Y243" s="41"/>
       <c r="Z243" s="41"/>
@@ -18120,10 +18117,10 @@
       <c r="P244" s="38"/>
       <c r="Q244" s="38"/>
       <c r="R244" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="S244" s="38" t="s">
         <v>441</v>
-      </c>
-      <c r="S244" s="38" t="s">
-        <v>442</v>
       </c>
       <c r="T244" s="37">
         <v>45322</v>
@@ -18132,7 +18129,7 @@
         <v>80</v>
       </c>
       <c r="V244" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="W244" s="38"/>
       <c r="X244" s="42"/>
@@ -18197,7 +18194,7 @@
       </c>
       <c r="W245" s="38"/>
       <c r="X245" s="42" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y245" s="41"/>
       <c r="Z245" s="41"/>
@@ -18305,10 +18302,10 @@
       <c r="P247" s="38"/>
       <c r="Q247" s="38"/>
       <c r="R247" s="38" t="s">
+        <v>440</v>
+      </c>
+      <c r="S247" s="38" t="s">
         <v>441</v>
-      </c>
-      <c r="S247" s="38" t="s">
-        <v>442</v>
       </c>
       <c r="T247" s="37">
         <v>45322</v>
@@ -18317,7 +18314,7 @@
         <v>80</v>
       </c>
       <c r="V247" s="38" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="W247" s="38"/>
       <c r="X247" s="42"/>
@@ -18390,7 +18387,102 @@
       <c r="AD248" s="41"/>
       <c r="AE248" s="41"/>
     </row>
+    <row r="249" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A249" s="37">
+        <v>45345</v>
+      </c>
+      <c r="B249" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C249" s="38"/>
+      <c r="D249" s="38"/>
+      <c r="E249" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="J249" s="38">
+        <v>66</v>
+      </c>
+      <c r="K249" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L249" s="38">
+        <v>37.815818999999998</v>
+      </c>
+      <c r="M249" s="38">
+        <v>-121.558995</v>
+      </c>
+      <c r="N249" s="38"/>
+      <c r="Q249" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="R249" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="S249" s="38" t="s">
+        <v>401</v>
+      </c>
+      <c r="T249" s="37">
+        <v>45301</v>
+      </c>
+      <c r="U249" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="V249" s="38" t="s">
+        <v>398</v>
+      </c>
+      <c r="W249" s="41"/>
+      <c r="X249" s="41"/>
+      <c r="Y249" s="41"/>
+    </row>
+    <row r="250" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A250" s="37">
+        <v>45345</v>
+      </c>
+      <c r="B250" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="C250" s="38"/>
+      <c r="D250" s="38"/>
+      <c r="E250" s="38" t="s">
+        <v>129</v>
+      </c>
+      <c r="J250" s="38">
+        <v>70</v>
+      </c>
+      <c r="K250" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="L250" s="38">
+        <v>37.815818999999998</v>
+      </c>
+      <c r="M250" s="38">
+        <v>-121.558995</v>
+      </c>
+      <c r="N250" s="38"/>
+      <c r="Q250" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="R250" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="S250" s="38" t="s">
+        <v>418</v>
+      </c>
+      <c r="T250" s="37">
+        <v>45315</v>
+      </c>
+      <c r="U250" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="V250" s="38" t="s">
+        <v>419</v>
+      </c>
+      <c r="W250" s="41"/>
+      <c r="X250" s="41"/>
+      <c r="Y250" s="41"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:X250" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X204">
     <sortCondition ref="A2:A204"/>
   </sortState>
@@ -18401,6 +18493,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D9A9DE233A30CB4EAECD318FD55378CC" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8fd2cacec9171f93eb894d0689f08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65146633-a755-433a-aacb-5024b6511b89" xmlns:ns3="d8e23be6-d007-4c2c-9265-7d9405abf22e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a569083f6831735b7a488ac820eb0384" ns2:_="" ns3:_="">
     <xsd:import namespace="65146633-a755-433a-aacb-5024b6511b89"/>
@@ -18635,17 +18738,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -18656,6 +18748,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4F8AF6-B64B-4962-81B5-D73EE7A1E0CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
+    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76D96E8C-3FF7-4769-9DB8-E43AB53278F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -18674,17 +18777,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4F8AF6-B64B-4962-81B5-D73EE7A1E0CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
-    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
updated with catch from april and may
</commit_message>
<xml_diff>
--- a/Running Delta Smelt Catch_2023-09-05.xlsx
+++ b/Running Delta Smelt Catch_2023-09-05.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/SmeltMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{38D2B3C1-DAF9-4126-B4FD-0E27163FBC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{219EFBEC-7B0E-4EE4-9063-C32692BBF937}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{38D2B3C1-DAF9-4126-B4FD-0E27163FBC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEB2348B-629E-4A4D-A2BC-E61B08AC0674}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3796" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4491" uniqueCount="527">
   <si>
     <t>Running Delta Smelt Catch Data Collected for the USFWS Delta Smelt Experimental Release Technical Team</t>
   </si>
@@ -1563,12 +1563,93 @@
   </si>
   <si>
     <t>Species ID confirmed by Rene Reyes</t>
+  </si>
+  <si>
+    <t>24-36-SSC04</t>
+  </si>
+  <si>
+    <t>24-37-SM05</t>
+  </si>
+  <si>
+    <t>24-37-SB03</t>
+  </si>
+  <si>
+    <t>24-37-SB07</t>
+  </si>
+  <si>
+    <t>24-37-SB11</t>
+  </si>
+  <si>
+    <t>24-37-SSC05</t>
+  </si>
+  <si>
+    <t>24-37-SSC02</t>
+  </si>
+  <si>
+    <t>24-37-SSC01</t>
+  </si>
+  <si>
+    <t>24-37-LSR04</t>
+  </si>
+  <si>
+    <t>24-37-SB10</t>
+  </si>
+  <si>
+    <t>24-38-LSR02</t>
+  </si>
+  <si>
+    <t>24-38-SM09</t>
+  </si>
+  <si>
+    <t>24-38-SB03</t>
+  </si>
+  <si>
+    <t>24-38-SSC03</t>
+  </si>
+  <si>
+    <t>24-38-SSC05</t>
+  </si>
+  <si>
+    <t>24-39-SB05</t>
+  </si>
+  <si>
+    <t>24-39-SSC01</t>
+  </si>
+  <si>
+    <t>24-39-SSC02</t>
+  </si>
+  <si>
+    <t>24-39-SSC04</t>
+  </si>
+  <si>
+    <t>24-39-SM01</t>
+  </si>
+  <si>
+    <t>24-39-LSR10</t>
+  </si>
+  <si>
+    <t>24-40-LSR04</t>
+  </si>
+  <si>
+    <t>24-40-LSR02</t>
+  </si>
+  <si>
+    <t>24-40-LSR03</t>
+  </si>
+  <si>
+    <t>24-40-SSC03</t>
+  </si>
+  <si>
+    <t>24-41-SSC02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1748,7 +1829,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1859,6 +1940,7 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2570,11 +2652,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
-  <dimension ref="A1:AE264"/>
+  <dimension ref="A1:AE403"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A244" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I272" sqref="I272"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A260" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G274" sqref="G274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -21224,6 +21306,4037 @@
       <c r="AC264" s="38"/>
       <c r="AD264" s="38"/>
       <c r="AE264" s="38"/>
+    </row>
+    <row r="265" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A265" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B265" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C265" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D265" t="s">
+        <v>501</v>
+      </c>
+      <c r="E265" t="s">
+        <v>221</v>
+      </c>
+      <c r="J265">
+        <v>10.6</v>
+      </c>
+      <c r="K265" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L265">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M265">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="266" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A266" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B266" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C266" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D266" t="s">
+        <v>501</v>
+      </c>
+      <c r="E266" t="s">
+        <v>221</v>
+      </c>
+      <c r="J266">
+        <v>10.7</v>
+      </c>
+      <c r="K266" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L266">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M266">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="267" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A267" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B267" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C267" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D267" t="s">
+        <v>501</v>
+      </c>
+      <c r="E267" t="s">
+        <v>221</v>
+      </c>
+      <c r="J267">
+        <v>11.7</v>
+      </c>
+      <c r="K267" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L267">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M267">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="268" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A268" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B268" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C268" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D268" t="s">
+        <v>501</v>
+      </c>
+      <c r="E268" t="s">
+        <v>221</v>
+      </c>
+      <c r="J268">
+        <v>11.7</v>
+      </c>
+      <c r="K268" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L268">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M268">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="269" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A269" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B269" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C269" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D269" t="s">
+        <v>501</v>
+      </c>
+      <c r="E269" t="s">
+        <v>221</v>
+      </c>
+      <c r="J269">
+        <v>12</v>
+      </c>
+      <c r="K269" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L269">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M269">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="270" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A270" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B270" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C270" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D270" t="s">
+        <v>501</v>
+      </c>
+      <c r="E270" t="s">
+        <v>221</v>
+      </c>
+      <c r="J270">
+        <v>12.1</v>
+      </c>
+      <c r="K270" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L270">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M270">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="271" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A271" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B271" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C271" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D271" t="s">
+        <v>501</v>
+      </c>
+      <c r="E271" t="s">
+        <v>221</v>
+      </c>
+      <c r="J271">
+        <v>12.1</v>
+      </c>
+      <c r="K271" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L271">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M271">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="272" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A272" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B272" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C272" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D272" t="s">
+        <v>501</v>
+      </c>
+      <c r="E272" t="s">
+        <v>221</v>
+      </c>
+      <c r="J272">
+        <v>12.1</v>
+      </c>
+      <c r="K272" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L272">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M272">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="273" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A273" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B273" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C273" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D273" t="s">
+        <v>501</v>
+      </c>
+      <c r="E273" t="s">
+        <v>221</v>
+      </c>
+      <c r="J273">
+        <v>12.4</v>
+      </c>
+      <c r="K273" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L273">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M273">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="274" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A274" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B274" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C274" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D274" t="s">
+        <v>501</v>
+      </c>
+      <c r="E274" t="s">
+        <v>221</v>
+      </c>
+      <c r="J274">
+        <v>12.6</v>
+      </c>
+      <c r="K274" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L274">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M274">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="275" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A275" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B275" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C275" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D275" t="s">
+        <v>501</v>
+      </c>
+      <c r="E275" t="s">
+        <v>221</v>
+      </c>
+      <c r="J275">
+        <v>13.4</v>
+      </c>
+      <c r="K275" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L275">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M275">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="276" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A276" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B276" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C276" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D276" t="s">
+        <v>501</v>
+      </c>
+      <c r="E276" t="s">
+        <v>221</v>
+      </c>
+      <c r="J276">
+        <v>13.8</v>
+      </c>
+      <c r="K276" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L276">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M276">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="277" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A277" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B277" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C277" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D277" t="s">
+        <v>501</v>
+      </c>
+      <c r="E277" t="s">
+        <v>221</v>
+      </c>
+      <c r="J277">
+        <v>13.9</v>
+      </c>
+      <c r="K277" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L277">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M277">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="278" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A278" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B278" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C278" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D278" t="s">
+        <v>501</v>
+      </c>
+      <c r="E278" t="s">
+        <v>221</v>
+      </c>
+      <c r="J278">
+        <v>14</v>
+      </c>
+      <c r="K278" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L278">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M278">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="279" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A279" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B279" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C279" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D279" t="s">
+        <v>501</v>
+      </c>
+      <c r="E279" t="s">
+        <v>221</v>
+      </c>
+      <c r="J279">
+        <v>14.1</v>
+      </c>
+      <c r="K279" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L279">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M279">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="280" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A280" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B280" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C280" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D280" t="s">
+        <v>501</v>
+      </c>
+      <c r="E280" t="s">
+        <v>221</v>
+      </c>
+      <c r="J280">
+        <v>14.1</v>
+      </c>
+      <c r="K280" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L280">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M280">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="281" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A281" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B281" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C281" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D281" t="s">
+        <v>501</v>
+      </c>
+      <c r="E281" t="s">
+        <v>221</v>
+      </c>
+      <c r="J281">
+        <v>14.4</v>
+      </c>
+      <c r="K281" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L281">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M281">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="282" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A282" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B282" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C282" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D282" t="s">
+        <v>501</v>
+      </c>
+      <c r="E282" t="s">
+        <v>221</v>
+      </c>
+      <c r="J282">
+        <v>14.5</v>
+      </c>
+      <c r="K282" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L282">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M282">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="283" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A283" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B283" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C283" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D283" t="s">
+        <v>501</v>
+      </c>
+      <c r="E283" t="s">
+        <v>221</v>
+      </c>
+      <c r="J283">
+        <v>14.7</v>
+      </c>
+      <c r="K283" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L283">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M283">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="284" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A284" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B284" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C284" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D284" t="s">
+        <v>501</v>
+      </c>
+      <c r="E284" t="s">
+        <v>221</v>
+      </c>
+      <c r="J284">
+        <v>14.7</v>
+      </c>
+      <c r="K284" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L284">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M284">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="285" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A285" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B285" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C285" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D285" t="s">
+        <v>501</v>
+      </c>
+      <c r="E285" t="s">
+        <v>221</v>
+      </c>
+      <c r="J285">
+        <v>15.1</v>
+      </c>
+      <c r="K285" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L285">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M285">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="286" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A286" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B286" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C286" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D286" t="s">
+        <v>501</v>
+      </c>
+      <c r="E286" t="s">
+        <v>221</v>
+      </c>
+      <c r="J286">
+        <v>15.6</v>
+      </c>
+      <c r="K286" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L286">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M286">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="287" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A287" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B287" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C287" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D287" t="s">
+        <v>501</v>
+      </c>
+      <c r="E287" t="s">
+        <v>221</v>
+      </c>
+      <c r="J287">
+        <v>16.5</v>
+      </c>
+      <c r="K287" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L287">
+        <v>38.563960000000002</v>
+      </c>
+      <c r="M287">
+        <v>-121.55369</v>
+      </c>
+    </row>
+    <row r="288" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A288" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B288" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C288" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D288" t="s">
+        <v>501</v>
+      </c>
+      <c r="E288" t="s">
+        <v>221</v>
+      </c>
+      <c r="J288">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K288" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L288">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M288">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="289" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A289" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B289" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C289" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D289" t="s">
+        <v>501</v>
+      </c>
+      <c r="E289" t="s">
+        <v>221</v>
+      </c>
+      <c r="J289">
+        <v>11.2</v>
+      </c>
+      <c r="K289" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L289">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M289">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="290" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A290" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B290" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C290" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D290" t="s">
+        <v>501</v>
+      </c>
+      <c r="E290" t="s">
+        <v>221</v>
+      </c>
+      <c r="J290">
+        <v>11.5</v>
+      </c>
+      <c r="K290" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L290">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M290">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="291" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A291" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B291" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C291" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D291" t="s">
+        <v>501</v>
+      </c>
+      <c r="E291" t="s">
+        <v>221</v>
+      </c>
+      <c r="J291">
+        <v>12.4</v>
+      </c>
+      <c r="K291" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L291">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M291">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="292" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A292" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B292" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C292" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D292" t="s">
+        <v>501</v>
+      </c>
+      <c r="E292" t="s">
+        <v>221</v>
+      </c>
+      <c r="J292">
+        <v>12.8</v>
+      </c>
+      <c r="K292" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L292">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M292">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="293" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A293" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B293" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C293" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D293" t="s">
+        <v>501</v>
+      </c>
+      <c r="E293" t="s">
+        <v>221</v>
+      </c>
+      <c r="J293">
+        <v>12.9</v>
+      </c>
+      <c r="K293" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L293">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M293">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="294" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A294" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B294" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C294" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D294" t="s">
+        <v>501</v>
+      </c>
+      <c r="E294" t="s">
+        <v>221</v>
+      </c>
+      <c r="J294">
+        <v>13</v>
+      </c>
+      <c r="K294" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L294">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M294">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="295" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A295" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B295" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C295" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D295" t="s">
+        <v>501</v>
+      </c>
+      <c r="E295" t="s">
+        <v>221</v>
+      </c>
+      <c r="J295">
+        <v>13.2</v>
+      </c>
+      <c r="K295" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L295">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M295">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="296" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A296" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B296" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C296" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D296" t="s">
+        <v>501</v>
+      </c>
+      <c r="E296" t="s">
+        <v>221</v>
+      </c>
+      <c r="J296">
+        <v>13.4</v>
+      </c>
+      <c r="K296" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L296">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M296">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A297" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B297" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C297" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D297" t="s">
+        <v>501</v>
+      </c>
+      <c r="E297" t="s">
+        <v>221</v>
+      </c>
+      <c r="J297">
+        <v>13.6</v>
+      </c>
+      <c r="K297" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L297">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M297">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="298" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A298" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B298" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C298" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D298" t="s">
+        <v>501</v>
+      </c>
+      <c r="E298" t="s">
+        <v>221</v>
+      </c>
+      <c r="J298">
+        <v>14</v>
+      </c>
+      <c r="K298" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L298">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M298">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="299" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A299" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B299" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C299" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D299" t="s">
+        <v>501</v>
+      </c>
+      <c r="E299" t="s">
+        <v>221</v>
+      </c>
+      <c r="J299">
+        <v>14.1</v>
+      </c>
+      <c r="K299" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L299">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M299">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="300" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A300" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B300" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C300" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D300" t="s">
+        <v>501</v>
+      </c>
+      <c r="E300" t="s">
+        <v>221</v>
+      </c>
+      <c r="J300">
+        <v>14.1</v>
+      </c>
+      <c r="K300" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L300">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M300">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="301" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A301" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B301" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C301" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D301" t="s">
+        <v>501</v>
+      </c>
+      <c r="E301" t="s">
+        <v>221</v>
+      </c>
+      <c r="J301">
+        <v>14.3</v>
+      </c>
+      <c r="K301" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L301">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M301">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="302" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A302" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B302" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C302" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D302" t="s">
+        <v>501</v>
+      </c>
+      <c r="E302" t="s">
+        <v>221</v>
+      </c>
+      <c r="J302">
+        <v>14.3</v>
+      </c>
+      <c r="K302" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L302">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M302">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="303" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A303" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B303" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C303" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D303" t="s">
+        <v>501</v>
+      </c>
+      <c r="E303" t="s">
+        <v>221</v>
+      </c>
+      <c r="J303">
+        <v>14.6</v>
+      </c>
+      <c r="K303" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L303">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M303">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="304" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A304" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B304" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C304" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D304" t="s">
+        <v>501</v>
+      </c>
+      <c r="E304" t="s">
+        <v>221</v>
+      </c>
+      <c r="J304">
+        <v>14.6</v>
+      </c>
+      <c r="K304" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L304">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M304">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="305" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A305" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B305" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C305" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D305" t="s">
+        <v>501</v>
+      </c>
+      <c r="E305" t="s">
+        <v>221</v>
+      </c>
+      <c r="J305">
+        <v>15.2</v>
+      </c>
+      <c r="K305" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L305">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M305">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="306" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A306" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B306" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C306" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D306" t="s">
+        <v>501</v>
+      </c>
+      <c r="E306" t="s">
+        <v>221</v>
+      </c>
+      <c r="J306">
+        <v>15.4</v>
+      </c>
+      <c r="K306" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L306">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M306">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="307" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A307" s="44">
+        <v>45387</v>
+      </c>
+      <c r="B307" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C307" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D307" t="s">
+        <v>501</v>
+      </c>
+      <c r="E307" t="s">
+        <v>221</v>
+      </c>
+      <c r="J307">
+        <v>18.5</v>
+      </c>
+      <c r="K307" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L307">
+        <v>38.564140000000002</v>
+      </c>
+      <c r="M307">
+        <v>-121.55392000000001</v>
+      </c>
+    </row>
+    <row r="308" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A308" s="44">
+        <v>45390</v>
+      </c>
+      <c r="B308" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C308" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D308" t="s">
+        <v>502</v>
+      </c>
+      <c r="E308" t="s">
+        <v>112</v>
+      </c>
+      <c r="J308">
+        <v>11.5</v>
+      </c>
+      <c r="K308" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L308">
+        <v>38.136949999999999</v>
+      </c>
+      <c r="M308">
+        <v>-122.06022</v>
+      </c>
+    </row>
+    <row r="309" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A309" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B309" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C309" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D309" t="s">
+        <v>503</v>
+      </c>
+      <c r="E309" t="s">
+        <v>89</v>
+      </c>
+      <c r="J309">
+        <v>7</v>
+      </c>
+      <c r="K309" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L309">
+        <v>38.032580000000003</v>
+      </c>
+      <c r="M309">
+        <v>-122.1326</v>
+      </c>
+    </row>
+    <row r="310" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A310" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B310" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C310" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D310" t="s">
+        <v>503</v>
+      </c>
+      <c r="E310" t="s">
+        <v>89</v>
+      </c>
+      <c r="J310">
+        <v>6</v>
+      </c>
+      <c r="K310" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L310">
+        <v>38.032519999999998</v>
+      </c>
+      <c r="M310">
+        <v>-122.13254999999999</v>
+      </c>
+    </row>
+    <row r="311" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A311" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B311" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C311" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D311" t="s">
+        <v>503</v>
+      </c>
+      <c r="E311" t="s">
+        <v>89</v>
+      </c>
+      <c r="J311">
+        <v>6</v>
+      </c>
+      <c r="K311" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L311">
+        <v>38.032519999999998</v>
+      </c>
+      <c r="M311">
+        <v>-122.13254999999999</v>
+      </c>
+    </row>
+    <row r="312" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A312" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B312" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C312" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D312" t="s">
+        <v>503</v>
+      </c>
+      <c r="E312" t="s">
+        <v>89</v>
+      </c>
+      <c r="J312">
+        <v>6.5</v>
+      </c>
+      <c r="K312" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L312">
+        <v>38.032519999999998</v>
+      </c>
+      <c r="M312">
+        <v>-122.13254999999999</v>
+      </c>
+    </row>
+    <row r="313" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A313" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B313" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C313" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D313" t="s">
+        <v>503</v>
+      </c>
+      <c r="E313" t="s">
+        <v>89</v>
+      </c>
+      <c r="J313">
+        <v>7.5</v>
+      </c>
+      <c r="K313" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L313">
+        <v>38.032519999999998</v>
+      </c>
+      <c r="M313">
+        <v>-122.13254999999999</v>
+      </c>
+    </row>
+    <row r="314" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A314" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B314" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C314" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D314" t="s">
+        <v>504</v>
+      </c>
+      <c r="E314" t="s">
+        <v>89</v>
+      </c>
+      <c r="J314">
+        <v>5.7</v>
+      </c>
+      <c r="K314" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L314">
+        <v>38.050910000000002</v>
+      </c>
+      <c r="M314">
+        <v>-122.08477999999999</v>
+      </c>
+    </row>
+    <row r="315" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A315" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B315" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C315" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D315" t="s">
+        <v>504</v>
+      </c>
+      <c r="E315" t="s">
+        <v>89</v>
+      </c>
+      <c r="J315">
+        <v>6.5</v>
+      </c>
+      <c r="K315" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L315">
+        <v>38.050910000000002</v>
+      </c>
+      <c r="M315">
+        <v>-122.08477999999999</v>
+      </c>
+    </row>
+    <row r="316" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A316" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B316" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C316" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D316" t="s">
+        <v>504</v>
+      </c>
+      <c r="E316" t="s">
+        <v>89</v>
+      </c>
+      <c r="J316">
+        <v>8.1</v>
+      </c>
+      <c r="K316" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L316">
+        <v>38.050910000000002</v>
+      </c>
+      <c r="M316">
+        <v>-122.08477999999999</v>
+      </c>
+    </row>
+    <row r="317" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A317" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B317" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C317" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D317" t="s">
+        <v>504</v>
+      </c>
+      <c r="E317" t="s">
+        <v>89</v>
+      </c>
+      <c r="J317">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="K317" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L317">
+        <v>38.050910000000002</v>
+      </c>
+      <c r="M317">
+        <v>-122.08477999999999</v>
+      </c>
+    </row>
+    <row r="318" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A318" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B318" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C318" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D318" t="s">
+        <v>504</v>
+      </c>
+      <c r="E318" t="s">
+        <v>89</v>
+      </c>
+      <c r="J318">
+        <v>9.5</v>
+      </c>
+      <c r="K318" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L318">
+        <v>38.050910000000002</v>
+      </c>
+      <c r="M318">
+        <v>-122.08477999999999</v>
+      </c>
+    </row>
+    <row r="319" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A319" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B319" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C319" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D319" t="s">
+        <v>504</v>
+      </c>
+      <c r="E319" t="s">
+        <v>89</v>
+      </c>
+      <c r="J319">
+        <v>10.7</v>
+      </c>
+      <c r="K319" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L319">
+        <v>38.050910000000002</v>
+      </c>
+      <c r="M319">
+        <v>-122.08477999999999</v>
+      </c>
+    </row>
+    <row r="320" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A320" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B320" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C320" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D320" t="s">
+        <v>505</v>
+      </c>
+      <c r="E320" t="s">
+        <v>89</v>
+      </c>
+      <c r="J320">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K320" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L320">
+        <v>38.046149999999997</v>
+      </c>
+      <c r="M320">
+        <v>-122.10866</v>
+      </c>
+    </row>
+    <row r="321" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A321" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B321" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C321" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D321" t="s">
+        <v>506</v>
+      </c>
+      <c r="E321" t="s">
+        <v>221</v>
+      </c>
+      <c r="J321">
+        <v>7.2</v>
+      </c>
+      <c r="K321" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L321">
+        <v>38.49783</v>
+      </c>
+      <c r="M321">
+        <v>-121.58484</v>
+      </c>
+    </row>
+    <row r="322" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A322" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B322" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C322" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D322" t="s">
+        <v>506</v>
+      </c>
+      <c r="E322" t="s">
+        <v>221</v>
+      </c>
+      <c r="J322">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K322" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L322">
+        <v>38.49783</v>
+      </c>
+      <c r="M322">
+        <v>-121.58484</v>
+      </c>
+    </row>
+    <row r="323" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A323" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B323" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C323" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D323" t="s">
+        <v>506</v>
+      </c>
+      <c r="E323" t="s">
+        <v>221</v>
+      </c>
+      <c r="J323">
+        <v>10</v>
+      </c>
+      <c r="K323" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L323">
+        <v>38.49783</v>
+      </c>
+      <c r="M323">
+        <v>-121.58484</v>
+      </c>
+    </row>
+    <row r="324" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A324" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B324" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C324" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D324" t="s">
+        <v>506</v>
+      </c>
+      <c r="E324" t="s">
+        <v>221</v>
+      </c>
+      <c r="J324">
+        <v>11.1</v>
+      </c>
+      <c r="K324" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L324">
+        <v>38.49783</v>
+      </c>
+      <c r="M324">
+        <v>-121.58484</v>
+      </c>
+    </row>
+    <row r="325" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A325" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B325" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C325" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D325" t="s">
+        <v>506</v>
+      </c>
+      <c r="E325" t="s">
+        <v>221</v>
+      </c>
+      <c r="J325">
+        <v>12</v>
+      </c>
+      <c r="K325" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L325">
+        <v>38.49783</v>
+      </c>
+      <c r="M325">
+        <v>-121.58484</v>
+      </c>
+    </row>
+    <row r="326" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A326" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B326" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C326" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D326" t="s">
+        <v>506</v>
+      </c>
+      <c r="E326" t="s">
+        <v>221</v>
+      </c>
+      <c r="J326">
+        <v>12.4</v>
+      </c>
+      <c r="K326" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L326">
+        <v>38.49783</v>
+      </c>
+      <c r="M326">
+        <v>-121.58484</v>
+      </c>
+    </row>
+    <row r="327" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A327" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B327" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C327" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D327" t="s">
+        <v>506</v>
+      </c>
+      <c r="E327" t="s">
+        <v>221</v>
+      </c>
+      <c r="J327">
+        <v>13.2</v>
+      </c>
+      <c r="K327" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L327">
+        <v>38.49783</v>
+      </c>
+      <c r="M327">
+        <v>-121.58484</v>
+      </c>
+    </row>
+    <row r="328" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A328" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B328" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C328" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D328" t="s">
+        <v>506</v>
+      </c>
+      <c r="E328" t="s">
+        <v>221</v>
+      </c>
+      <c r="J328">
+        <v>11.3</v>
+      </c>
+      <c r="K328" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L328">
+        <v>38.49897</v>
+      </c>
+      <c r="M328">
+        <v>-121.58477000000001</v>
+      </c>
+    </row>
+    <row r="329" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A329" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B329" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C329" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D329" t="s">
+        <v>506</v>
+      </c>
+      <c r="E329" t="s">
+        <v>221</v>
+      </c>
+      <c r="J329">
+        <v>11.8</v>
+      </c>
+      <c r="K329" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L329">
+        <v>38.49897</v>
+      </c>
+      <c r="M329">
+        <v>-121.58477000000001</v>
+      </c>
+    </row>
+    <row r="330" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A330" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B330" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C330" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D330" t="s">
+        <v>506</v>
+      </c>
+      <c r="E330" t="s">
+        <v>221</v>
+      </c>
+      <c r="J330">
+        <v>12.5</v>
+      </c>
+      <c r="K330" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L330">
+        <v>38.49897</v>
+      </c>
+      <c r="M330">
+        <v>-121.58477000000001</v>
+      </c>
+    </row>
+    <row r="331" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A331" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B331" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C331" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D331" t="s">
+        <v>506</v>
+      </c>
+      <c r="E331" t="s">
+        <v>221</v>
+      </c>
+      <c r="J331">
+        <v>13.3</v>
+      </c>
+      <c r="K331" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L331">
+        <v>38.49897</v>
+      </c>
+      <c r="M331">
+        <v>-121.58477000000001</v>
+      </c>
+    </row>
+    <row r="332" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A332" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B332" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C332" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D332" t="s">
+        <v>507</v>
+      </c>
+      <c r="E332" t="s">
+        <v>221</v>
+      </c>
+      <c r="J332">
+        <v>11.6</v>
+      </c>
+      <c r="K332" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L332">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M332">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="333" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A333" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B333" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C333" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D333" t="s">
+        <v>507</v>
+      </c>
+      <c r="E333" t="s">
+        <v>221</v>
+      </c>
+      <c r="J333">
+        <v>12.6</v>
+      </c>
+      <c r="K333" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L333">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M333">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="334" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A334" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B334" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C334" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D334" t="s">
+        <v>507</v>
+      </c>
+      <c r="E334" t="s">
+        <v>221</v>
+      </c>
+      <c r="J334">
+        <v>13</v>
+      </c>
+      <c r="K334" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L334">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M334">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="335" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A335" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B335" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C335" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D335" t="s">
+        <v>507</v>
+      </c>
+      <c r="E335" t="s">
+        <v>221</v>
+      </c>
+      <c r="J335">
+        <v>13.2</v>
+      </c>
+      <c r="K335" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L335">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M335">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="336" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A336" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B336" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C336" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D336" t="s">
+        <v>507</v>
+      </c>
+      <c r="E336" t="s">
+        <v>221</v>
+      </c>
+      <c r="J336">
+        <v>13.3</v>
+      </c>
+      <c r="K336" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L336">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M336">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="337" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A337" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B337" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C337" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D337" t="s">
+        <v>507</v>
+      </c>
+      <c r="E337" t="s">
+        <v>221</v>
+      </c>
+      <c r="J337">
+        <v>13.9</v>
+      </c>
+      <c r="K337" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L337">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M337">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="338" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A338" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B338" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C338" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D338" t="s">
+        <v>507</v>
+      </c>
+      <c r="E338" t="s">
+        <v>221</v>
+      </c>
+      <c r="J338">
+        <v>14</v>
+      </c>
+      <c r="K338" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L338">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M338">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="339" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A339" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B339" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C339" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D339" t="s">
+        <v>507</v>
+      </c>
+      <c r="E339" t="s">
+        <v>221</v>
+      </c>
+      <c r="J339">
+        <v>14.2</v>
+      </c>
+      <c r="K339" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L339">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M339">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="340" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A340" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B340" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C340" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D340" t="s">
+        <v>507</v>
+      </c>
+      <c r="E340" t="s">
+        <v>221</v>
+      </c>
+      <c r="J340">
+        <v>14.3</v>
+      </c>
+      <c r="K340" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L340">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M340">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A341" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B341" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C341" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D341" t="s">
+        <v>507</v>
+      </c>
+      <c r="E341" t="s">
+        <v>221</v>
+      </c>
+      <c r="J341">
+        <v>14.5</v>
+      </c>
+      <c r="K341" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L341">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M341">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A342" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B342" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C342" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D342" t="s">
+        <v>507</v>
+      </c>
+      <c r="E342" t="s">
+        <v>221</v>
+      </c>
+      <c r="J342">
+        <v>14.6</v>
+      </c>
+      <c r="K342" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L342">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M342">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A343" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B343" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C343" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D343" t="s">
+        <v>507</v>
+      </c>
+      <c r="E343" t="s">
+        <v>221</v>
+      </c>
+      <c r="J343">
+        <v>14.8</v>
+      </c>
+      <c r="K343" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L343">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M343">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A344" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B344" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C344" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D344" t="s">
+        <v>507</v>
+      </c>
+      <c r="E344" t="s">
+        <v>221</v>
+      </c>
+      <c r="J344">
+        <v>15</v>
+      </c>
+      <c r="K344" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L344">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M344">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A345" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B345" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C345" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D345" t="s">
+        <v>507</v>
+      </c>
+      <c r="E345" t="s">
+        <v>221</v>
+      </c>
+      <c r="J345">
+        <v>15.1</v>
+      </c>
+      <c r="K345" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L345">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M345">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A346" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B346" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C346" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D346" t="s">
+        <v>507</v>
+      </c>
+      <c r="E346" t="s">
+        <v>221</v>
+      </c>
+      <c r="J346">
+        <v>15.3</v>
+      </c>
+      <c r="K346" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L346">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M346">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A347" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B347" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C347" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D347" t="s">
+        <v>507</v>
+      </c>
+      <c r="E347" t="s">
+        <v>221</v>
+      </c>
+      <c r="J347">
+        <v>15.8</v>
+      </c>
+      <c r="K347" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L347">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M347">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A348" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B348" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C348" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D348" t="s">
+        <v>507</v>
+      </c>
+      <c r="E348" t="s">
+        <v>221</v>
+      </c>
+      <c r="J348">
+        <v>15.9</v>
+      </c>
+      <c r="K348" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L348">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M348">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A349" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B349" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C349" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D349" t="s">
+        <v>507</v>
+      </c>
+      <c r="E349" t="s">
+        <v>221</v>
+      </c>
+      <c r="J349">
+        <v>16</v>
+      </c>
+      <c r="K349" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L349">
+        <v>38.479680000000002</v>
+      </c>
+      <c r="M349">
+        <v>-121.58496</v>
+      </c>
+    </row>
+    <row r="350" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A350" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B350" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C350" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D350" t="s">
+        <v>507</v>
+      </c>
+      <c r="E350" t="s">
+        <v>221</v>
+      </c>
+      <c r="J350">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K350" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L350">
+        <v>38.479599999999998</v>
+      </c>
+      <c r="M350">
+        <v>-121.58499</v>
+      </c>
+    </row>
+    <row r="351" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A351" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B351" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C351" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D351" t="s">
+        <v>507</v>
+      </c>
+      <c r="E351" t="s">
+        <v>221</v>
+      </c>
+      <c r="J351">
+        <v>12</v>
+      </c>
+      <c r="K351" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L351">
+        <v>38.479599999999998</v>
+      </c>
+      <c r="M351">
+        <v>-121.58499</v>
+      </c>
+    </row>
+    <row r="352" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A352" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B352" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C352" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D352" t="s">
+        <v>507</v>
+      </c>
+      <c r="E352" t="s">
+        <v>221</v>
+      </c>
+      <c r="J352">
+        <v>12.2</v>
+      </c>
+      <c r="K352" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L352">
+        <v>38.479599999999998</v>
+      </c>
+      <c r="M352">
+        <v>-121.58499</v>
+      </c>
+    </row>
+    <row r="353" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A353" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B353" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C353" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D353" t="s">
+        <v>507</v>
+      </c>
+      <c r="E353" t="s">
+        <v>221</v>
+      </c>
+      <c r="J353">
+        <v>13</v>
+      </c>
+      <c r="K353" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L353">
+        <v>38.479599999999998</v>
+      </c>
+      <c r="M353">
+        <v>-121.58499</v>
+      </c>
+    </row>
+    <row r="354" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A354" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B354" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C354" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D354" t="s">
+        <v>507</v>
+      </c>
+      <c r="E354" t="s">
+        <v>221</v>
+      </c>
+      <c r="J354">
+        <v>13</v>
+      </c>
+      <c r="K354" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L354">
+        <v>38.479599999999998</v>
+      </c>
+      <c r="M354">
+        <v>-121.58499</v>
+      </c>
+    </row>
+    <row r="355" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A355" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B355" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C355" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D355" t="s">
+        <v>508</v>
+      </c>
+      <c r="E355" t="s">
+        <v>83</v>
+      </c>
+      <c r="J355">
+        <v>13.2</v>
+      </c>
+      <c r="K355" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L355">
+        <v>38.464799999999997</v>
+      </c>
+      <c r="M355">
+        <v>-121.58785</v>
+      </c>
+    </row>
+    <row r="356" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A356" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B356" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C356" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D356" t="s">
+        <v>508</v>
+      </c>
+      <c r="E356" t="s">
+        <v>83</v>
+      </c>
+      <c r="J356">
+        <v>13.4</v>
+      </c>
+      <c r="K356" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L356">
+        <v>38.464799999999997</v>
+      </c>
+      <c r="M356">
+        <v>-121.58785</v>
+      </c>
+    </row>
+    <row r="357" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A357" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B357" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C357" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D357" t="s">
+        <v>508</v>
+      </c>
+      <c r="E357" t="s">
+        <v>83</v>
+      </c>
+      <c r="J357">
+        <v>14.4</v>
+      </c>
+      <c r="K357" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L357">
+        <v>38.464799999999997</v>
+      </c>
+      <c r="M357">
+        <v>-121.58785</v>
+      </c>
+    </row>
+    <row r="358" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A358" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B358" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C358" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D358" t="s">
+        <v>508</v>
+      </c>
+      <c r="E358" t="s">
+        <v>83</v>
+      </c>
+      <c r="J358">
+        <v>14.9</v>
+      </c>
+      <c r="K358" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L358">
+        <v>38.464799999999997</v>
+      </c>
+      <c r="M358">
+        <v>-121.58785</v>
+      </c>
+    </row>
+    <row r="359" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A359" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B359" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C359" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D359" t="s">
+        <v>508</v>
+      </c>
+      <c r="E359" t="s">
+        <v>83</v>
+      </c>
+      <c r="J359">
+        <v>15.2</v>
+      </c>
+      <c r="K359" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L359">
+        <v>38.464799999999997</v>
+      </c>
+      <c r="M359">
+        <v>-121.58785</v>
+      </c>
+    </row>
+    <row r="360" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A360" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B360" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C360" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D360" t="s">
+        <v>508</v>
+      </c>
+      <c r="E360" t="s">
+        <v>83</v>
+      </c>
+      <c r="J360">
+        <v>15.8</v>
+      </c>
+      <c r="K360" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L360">
+        <v>38.464799999999997</v>
+      </c>
+      <c r="M360">
+        <v>-121.58785</v>
+      </c>
+    </row>
+    <row r="361" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A361" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B361" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C361" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D361" t="s">
+        <v>508</v>
+      </c>
+      <c r="E361" t="s">
+        <v>83</v>
+      </c>
+      <c r="J361">
+        <v>12.8</v>
+      </c>
+      <c r="K361" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L361">
+        <v>38.465339999999998</v>
+      </c>
+      <c r="M361">
+        <v>-121.58781999999999</v>
+      </c>
+    </row>
+    <row r="362" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A362" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B362" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C362" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D362" t="s">
+        <v>508</v>
+      </c>
+      <c r="E362" t="s">
+        <v>83</v>
+      </c>
+      <c r="J362">
+        <v>14</v>
+      </c>
+      <c r="K362" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L362">
+        <v>38.465339999999998</v>
+      </c>
+      <c r="M362">
+        <v>-121.58781999999999</v>
+      </c>
+    </row>
+    <row r="363" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A363" s="44">
+        <v>45391</v>
+      </c>
+      <c r="B363" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C363" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D363" t="s">
+        <v>508</v>
+      </c>
+      <c r="E363" t="s">
+        <v>83</v>
+      </c>
+      <c r="J363">
+        <v>16</v>
+      </c>
+      <c r="K363" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L363">
+        <v>38.465339999999998</v>
+      </c>
+      <c r="M363">
+        <v>-121.58781999999999</v>
+      </c>
+    </row>
+    <row r="364" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A364" s="44">
+        <v>45392</v>
+      </c>
+      <c r="B364" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C364" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D364" t="s">
+        <v>509</v>
+      </c>
+      <c r="E364" t="s">
+        <v>90</v>
+      </c>
+      <c r="J364">
+        <v>9.6</v>
+      </c>
+      <c r="K364" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L364">
+        <v>38.07302</v>
+      </c>
+      <c r="M364">
+        <v>-121.77419999999999</v>
+      </c>
+    </row>
+    <row r="365" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A365" s="44">
+        <v>45393</v>
+      </c>
+      <c r="B365" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C365" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D365" t="s">
+        <v>510</v>
+      </c>
+      <c r="E365" t="s">
+        <v>150</v>
+      </c>
+      <c r="J365">
+        <v>6.2</v>
+      </c>
+      <c r="K365" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L365">
+        <v>38.054250000000003</v>
+      </c>
+      <c r="M365">
+        <v>-121.95818</v>
+      </c>
+    </row>
+    <row r="366" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A366" s="44">
+        <v>45393</v>
+      </c>
+      <c r="B366" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C366" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D366" t="s">
+        <v>510</v>
+      </c>
+      <c r="E366" t="s">
+        <v>150</v>
+      </c>
+      <c r="J366">
+        <v>7.1</v>
+      </c>
+      <c r="K366" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L366">
+        <v>38.054250000000003</v>
+      </c>
+      <c r="M366">
+        <v>-121.95818</v>
+      </c>
+    </row>
+    <row r="367" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A367" s="44">
+        <v>45393</v>
+      </c>
+      <c r="B367" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C367" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D367" t="s">
+        <v>510</v>
+      </c>
+      <c r="E367" t="s">
+        <v>150</v>
+      </c>
+      <c r="J367">
+        <v>7.6</v>
+      </c>
+      <c r="K367" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L367">
+        <v>38.054250000000003</v>
+      </c>
+      <c r="M367">
+        <v>-121.95818</v>
+      </c>
+    </row>
+    <row r="368" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A368" s="44">
+        <v>45393</v>
+      </c>
+      <c r="B368" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C368" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D368" t="s">
+        <v>510</v>
+      </c>
+      <c r="E368" t="s">
+        <v>150</v>
+      </c>
+      <c r="J368">
+        <v>7.7</v>
+      </c>
+      <c r="K368" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L368">
+        <v>38.054250000000003</v>
+      </c>
+      <c r="M368">
+        <v>-121.95818</v>
+      </c>
+    </row>
+    <row r="369" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A369" s="44">
+        <v>45393</v>
+      </c>
+      <c r="B369" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C369" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D369" t="s">
+        <v>510</v>
+      </c>
+      <c r="E369" t="s">
+        <v>150</v>
+      </c>
+      <c r="J369">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K369" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L369">
+        <v>38.054250000000003</v>
+      </c>
+      <c r="M369">
+        <v>-121.95818</v>
+      </c>
+    </row>
+    <row r="370" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A370" s="44">
+        <v>45393</v>
+      </c>
+      <c r="B370" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C370" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D370" t="s">
+        <v>510</v>
+      </c>
+      <c r="E370" t="s">
+        <v>150</v>
+      </c>
+      <c r="J370">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K370" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L370">
+        <v>38.054250000000003</v>
+      </c>
+      <c r="M370">
+        <v>-121.95818</v>
+      </c>
+    </row>
+    <row r="371" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A371" s="44">
+        <v>45393</v>
+      </c>
+      <c r="B371" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C371" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D371" t="s">
+        <v>510</v>
+      </c>
+      <c r="E371" t="s">
+        <v>150</v>
+      </c>
+      <c r="J371">
+        <v>7</v>
+      </c>
+      <c r="K371" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L371">
+        <v>38.054200000000002</v>
+      </c>
+      <c r="M371">
+        <v>-121.95825000000001</v>
+      </c>
+    </row>
+    <row r="372" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A372" s="44">
+        <v>45393</v>
+      </c>
+      <c r="B372" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C372" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D372" t="s">
+        <v>510</v>
+      </c>
+      <c r="E372" t="s">
+        <v>150</v>
+      </c>
+      <c r="J372">
+        <v>9</v>
+      </c>
+      <c r="K372" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L372">
+        <v>38.054200000000002</v>
+      </c>
+      <c r="M372">
+        <v>-121.95825000000001</v>
+      </c>
+    </row>
+    <row r="373" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A373" s="44">
+        <v>45397</v>
+      </c>
+      <c r="B373" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C373" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D373" t="s">
+        <v>511</v>
+      </c>
+      <c r="E373" t="s">
+        <v>84</v>
+      </c>
+      <c r="J373">
+        <v>12</v>
+      </c>
+      <c r="K373" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L373">
+        <v>38.111620000000002</v>
+      </c>
+      <c r="M373">
+        <v>-121.7099</v>
+      </c>
+    </row>
+    <row r="374" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A374" s="44">
+        <v>45398</v>
+      </c>
+      <c r="B374" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C374" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D374" t="s">
+        <v>512</v>
+      </c>
+      <c r="E374" t="s">
+        <v>112</v>
+      </c>
+      <c r="J374">
+        <v>9</v>
+      </c>
+      <c r="K374" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L374">
+        <v>38.155259999999998</v>
+      </c>
+      <c r="M374">
+        <v>-122.0527</v>
+      </c>
+    </row>
+    <row r="375" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A375" s="44">
+        <v>45399</v>
+      </c>
+      <c r="B375" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C375" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D375" t="s">
+        <v>513</v>
+      </c>
+      <c r="E375" t="s">
+        <v>89</v>
+      </c>
+      <c r="J375">
+        <v>7.6</v>
+      </c>
+      <c r="K375" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L375">
+        <v>38.091889999999999</v>
+      </c>
+      <c r="M375">
+        <v>-122.07877000000001</v>
+      </c>
+    </row>
+    <row r="376" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A376" s="44">
+        <v>45399</v>
+      </c>
+      <c r="B376" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C376" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D376" t="s">
+        <v>514</v>
+      </c>
+      <c r="E376" t="s">
+        <v>83</v>
+      </c>
+      <c r="J376">
+        <v>6.5</v>
+      </c>
+      <c r="K376" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L376">
+        <v>38.022261999999998</v>
+      </c>
+      <c r="M376">
+        <v>-121.67391000000001</v>
+      </c>
+    </row>
+    <row r="377" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A377" s="44">
+        <v>45399</v>
+      </c>
+      <c r="B377" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C377" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D377" t="s">
+        <v>514</v>
+      </c>
+      <c r="E377" t="s">
+        <v>83</v>
+      </c>
+      <c r="J377">
+        <v>7.8</v>
+      </c>
+      <c r="K377" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L377">
+        <v>38.022261999999998</v>
+      </c>
+      <c r="M377">
+        <v>-121.67391000000001</v>
+      </c>
+    </row>
+    <row r="378" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A378" s="44">
+        <v>45399</v>
+      </c>
+      <c r="B378" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C378" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D378" t="s">
+        <v>514</v>
+      </c>
+      <c r="E378" t="s">
+        <v>83</v>
+      </c>
+      <c r="J378">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K378" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L378">
+        <v>38.022261999999998</v>
+      </c>
+      <c r="M378">
+        <v>-121.67391000000001</v>
+      </c>
+    </row>
+    <row r="379" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A379" s="44">
+        <v>45399</v>
+      </c>
+      <c r="B379" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C379" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D379" t="s">
+        <v>515</v>
+      </c>
+      <c r="E379" t="s">
+        <v>83</v>
+      </c>
+      <c r="J379">
+        <v>9.5</v>
+      </c>
+      <c r="K379" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L379">
+        <v>38.253230000000002</v>
+      </c>
+      <c r="M379">
+        <v>-121.66818000000001</v>
+      </c>
+    </row>
+    <row r="380" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A380" s="44">
+        <v>45399</v>
+      </c>
+      <c r="B380" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C380" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D380" t="s">
+        <v>515</v>
+      </c>
+      <c r="E380" t="s">
+        <v>83</v>
+      </c>
+      <c r="J380">
+        <v>11.5</v>
+      </c>
+      <c r="K380" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L380">
+        <v>38.253230000000002</v>
+      </c>
+      <c r="M380">
+        <v>-121.66818000000001</v>
+      </c>
+    </row>
+    <row r="381" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A381" s="44">
+        <v>45405</v>
+      </c>
+      <c r="B381" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C381" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D381" t="s">
+        <v>516</v>
+      </c>
+      <c r="E381" t="s">
+        <v>89</v>
+      </c>
+      <c r="J381">
+        <v>7.1</v>
+      </c>
+      <c r="K381" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L381">
+        <v>38.061160000000001</v>
+      </c>
+      <c r="M381">
+        <v>-122.05566</v>
+      </c>
+    </row>
+    <row r="382" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A382" s="44">
+        <v>45405</v>
+      </c>
+      <c r="B382" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C382" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D382" t="s">
+        <v>516</v>
+      </c>
+      <c r="E382" t="s">
+        <v>89</v>
+      </c>
+      <c r="J382">
+        <v>7.9</v>
+      </c>
+      <c r="K382" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L382">
+        <v>38.061160000000001</v>
+      </c>
+      <c r="M382">
+        <v>-122.05566</v>
+      </c>
+    </row>
+    <row r="383" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A383" s="44">
+        <v>45405</v>
+      </c>
+      <c r="B383" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C383" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D383" t="s">
+        <v>516</v>
+      </c>
+      <c r="E383" t="s">
+        <v>89</v>
+      </c>
+      <c r="J383">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="K383" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L383">
+        <v>38.061160000000001</v>
+      </c>
+      <c r="M383">
+        <v>-122.05566</v>
+      </c>
+    </row>
+    <row r="384" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A384" s="44">
+        <v>45405</v>
+      </c>
+      <c r="B384" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C384" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D384" t="s">
+        <v>516</v>
+      </c>
+      <c r="E384" t="s">
+        <v>89</v>
+      </c>
+      <c r="J384">
+        <v>7.1</v>
+      </c>
+      <c r="K384" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L384">
+        <v>38.061149999999998</v>
+      </c>
+      <c r="M384">
+        <v>-122.05544</v>
+      </c>
+    </row>
+    <row r="385" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A385" s="44">
+        <v>45405</v>
+      </c>
+      <c r="B385" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C385" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D385" t="s">
+        <v>516</v>
+      </c>
+      <c r="E385" t="s">
+        <v>89</v>
+      </c>
+      <c r="J385">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K385" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L385">
+        <v>38.061149999999998</v>
+      </c>
+      <c r="M385">
+        <v>-122.05544</v>
+      </c>
+    </row>
+    <row r="386" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A386" s="44">
+        <v>45406</v>
+      </c>
+      <c r="B386" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C386" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D386" t="s">
+        <v>517</v>
+      </c>
+      <c r="E386" t="s">
+        <v>83</v>
+      </c>
+      <c r="J386">
+        <v>7.1</v>
+      </c>
+      <c r="K386" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L386">
+        <v>38.345239999999997</v>
+      </c>
+      <c r="M386">
+        <v>-121.64274</v>
+      </c>
+    </row>
+    <row r="387" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A387" s="44">
+        <v>45406</v>
+      </c>
+      <c r="B387" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C387" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D387" t="s">
+        <v>517</v>
+      </c>
+      <c r="E387" t="s">
+        <v>83</v>
+      </c>
+      <c r="J387">
+        <v>8.4</v>
+      </c>
+      <c r="K387" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L387">
+        <v>38.345239999999997</v>
+      </c>
+      <c r="M387">
+        <v>-121.64274</v>
+      </c>
+    </row>
+    <row r="388" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A388" s="44">
+        <v>45406</v>
+      </c>
+      <c r="B388" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C388" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D388" t="s">
+        <v>517</v>
+      </c>
+      <c r="E388" t="s">
+        <v>83</v>
+      </c>
+      <c r="J388">
+        <v>26</v>
+      </c>
+      <c r="K388" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L388">
+        <v>38.345239999999997</v>
+      </c>
+      <c r="M388">
+        <v>-121.64274</v>
+      </c>
+    </row>
+    <row r="389" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A389" s="44">
+        <v>45406</v>
+      </c>
+      <c r="B389" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C389" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D389" t="s">
+        <v>518</v>
+      </c>
+      <c r="E389" t="s">
+        <v>83</v>
+      </c>
+      <c r="J389">
+        <v>6</v>
+      </c>
+      <c r="K389" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L389">
+        <v>38.267209999999999</v>
+      </c>
+      <c r="M389">
+        <v>-121.66372</v>
+      </c>
+    </row>
+    <row r="390" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A390" s="44">
+        <v>45406</v>
+      </c>
+      <c r="B390" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C390" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D390" t="s">
+        <v>519</v>
+      </c>
+      <c r="E390" t="s">
+        <v>221</v>
+      </c>
+      <c r="J390">
+        <v>9.4</v>
+      </c>
+      <c r="K390" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L390">
+        <v>38.491970000000002</v>
+      </c>
+      <c r="M390">
+        <v>-121.83920000000001</v>
+      </c>
+    </row>
+    <row r="391" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A391" s="44">
+        <v>45406</v>
+      </c>
+      <c r="B391" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C391" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D391" t="s">
+        <v>519</v>
+      </c>
+      <c r="E391" t="s">
+        <v>221</v>
+      </c>
+      <c r="J391">
+        <v>10.9</v>
+      </c>
+      <c r="K391" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L391">
+        <v>38.491970000000002</v>
+      </c>
+      <c r="M391">
+        <v>-121.83920000000001</v>
+      </c>
+    </row>
+    <row r="392" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A392" s="44">
+        <v>45407</v>
+      </c>
+      <c r="B392" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C392" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D392" t="s">
+        <v>520</v>
+      </c>
+      <c r="E392" t="s">
+        <v>112</v>
+      </c>
+      <c r="J392">
+        <v>10.7</v>
+      </c>
+      <c r="K392" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L392">
+        <v>38.169739999999997</v>
+      </c>
+      <c r="M392">
+        <v>-122.02802</v>
+      </c>
+    </row>
+    <row r="393" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A393" s="44">
+        <v>45407</v>
+      </c>
+      <c r="B393" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C393" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D393" t="s">
+        <v>520</v>
+      </c>
+      <c r="E393" t="s">
+        <v>112</v>
+      </c>
+      <c r="J393">
+        <v>12</v>
+      </c>
+      <c r="K393" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L393">
+        <v>38.169739999999997</v>
+      </c>
+      <c r="M393">
+        <v>-122.02802</v>
+      </c>
+    </row>
+    <row r="394" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A394" s="44">
+        <v>45407</v>
+      </c>
+      <c r="B394" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C394" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D394" t="s">
+        <v>520</v>
+      </c>
+      <c r="E394" t="s">
+        <v>112</v>
+      </c>
+      <c r="J394">
+        <v>13.3</v>
+      </c>
+      <c r="K394" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L394">
+        <v>38.169739999999997</v>
+      </c>
+      <c r="M394">
+        <v>-122.02802</v>
+      </c>
+    </row>
+    <row r="395" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A395" s="44">
+        <v>45407</v>
+      </c>
+      <c r="B395" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C395" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D395" t="s">
+        <v>521</v>
+      </c>
+      <c r="E395" t="s">
+        <v>84</v>
+      </c>
+      <c r="J395">
+        <v>10.8</v>
+      </c>
+      <c r="K395" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L395">
+        <v>38.165309999999998</v>
+      </c>
+      <c r="M395">
+        <v>-121.68103000000001</v>
+      </c>
+    </row>
+    <row r="396" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A396" s="44">
+        <v>45411</v>
+      </c>
+      <c r="B396" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C396" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D396" t="s">
+        <v>522</v>
+      </c>
+      <c r="E396" t="s">
+        <v>90</v>
+      </c>
+      <c r="J396">
+        <v>7.8</v>
+      </c>
+      <c r="K396" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L396">
+        <v>38.05442</v>
+      </c>
+      <c r="M396">
+        <v>-121.79924</v>
+      </c>
+    </row>
+    <row r="397" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A397" s="44">
+        <v>45411</v>
+      </c>
+      <c r="B397" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C397" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D397" t="s">
+        <v>523</v>
+      </c>
+      <c r="E397" t="s">
+        <v>84</v>
+      </c>
+      <c r="J397">
+        <v>10.5</v>
+      </c>
+      <c r="K397" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L397">
+        <v>38.140639999999998</v>
+      </c>
+      <c r="M397">
+        <v>-121.69403</v>
+      </c>
+    </row>
+    <row r="398" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A398" s="44">
+        <v>45411</v>
+      </c>
+      <c r="B398" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C398" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D398" t="s">
+        <v>523</v>
+      </c>
+      <c r="E398" t="s">
+        <v>84</v>
+      </c>
+      <c r="J398">
+        <v>8.5</v>
+      </c>
+      <c r="K398" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L398">
+        <v>38.140509999999999</v>
+      </c>
+      <c r="M398">
+        <v>-121.69412</v>
+      </c>
+    </row>
+    <row r="399" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A399" s="44">
+        <v>45411</v>
+      </c>
+      <c r="B399" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C399" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D399" t="s">
+        <v>524</v>
+      </c>
+      <c r="E399" t="s">
+        <v>84</v>
+      </c>
+      <c r="J399">
+        <v>7</v>
+      </c>
+      <c r="K399" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L399">
+        <v>38.171109999999999</v>
+      </c>
+      <c r="M399">
+        <v>-121.67536</v>
+      </c>
+    </row>
+    <row r="400" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A400" s="44">
+        <v>45411</v>
+      </c>
+      <c r="B400" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C400" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D400" t="s">
+        <v>524</v>
+      </c>
+      <c r="E400" t="s">
+        <v>84</v>
+      </c>
+      <c r="J400">
+        <v>8.1</v>
+      </c>
+      <c r="K400" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L400">
+        <v>38.171109999999999</v>
+      </c>
+      <c r="M400">
+        <v>-121.67536</v>
+      </c>
+    </row>
+    <row r="401" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A401" s="44">
+        <v>45414</v>
+      </c>
+      <c r="B401" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C401" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D401" t="s">
+        <v>525</v>
+      </c>
+      <c r="E401" t="s">
+        <v>83</v>
+      </c>
+      <c r="J401">
+        <v>12.5</v>
+      </c>
+      <c r="K401" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L401">
+        <v>38.210650000000001</v>
+      </c>
+      <c r="M401">
+        <v>-121.66464000000001</v>
+      </c>
+    </row>
+    <row r="402" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A402" s="44">
+        <v>45419</v>
+      </c>
+      <c r="B402" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C402" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D402" t="s">
+        <v>526</v>
+      </c>
+      <c r="E402" t="s">
+        <v>83</v>
+      </c>
+      <c r="J402">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K402" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L402">
+        <v>38.216810000000002</v>
+      </c>
+      <c r="M402">
+        <v>-121.66967</v>
+      </c>
+    </row>
+    <row r="403" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A403" s="44">
+        <v>45419</v>
+      </c>
+      <c r="B403" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C403" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D403" t="s">
+        <v>526</v>
+      </c>
+      <c r="E403" t="s">
+        <v>83</v>
+      </c>
+      <c r="J403">
+        <v>11.8</v>
+      </c>
+      <c r="K403" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L403">
+        <v>38.216810000000002</v>
+      </c>
+      <c r="M403">
+        <v>-121.66967</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AE254" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}"/>
@@ -21476,15 +25589,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
@@ -21517,6 +25621,15 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76D96E8C-3FF7-4769-9DB8-E43AB53278F6}">
   <ds:schemaRefs>
@@ -21537,14 +25650,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4F8AF6-B64B-4962-81B5-D73EE7A1E0CA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -21553,4 +25658,12 @@
     <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
June 10th catch update
</commit_message>
<xml_diff>
--- a/Running Delta Smelt Catch_2023-09-05.xlsx
+++ b/Running Delta Smelt Catch_2023-09-05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/SmeltMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="8_{38D2B3C1-DAF9-4126-B4FD-0E27163FBC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25E7ECD2-2938-4D85-A234-0FBDA0021711}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{38D2B3C1-DAF9-4126-B4FD-0E27163FBC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BAB5A50-7168-4427-908C-1B0D06A5CEEB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="12" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4596" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4621" uniqueCount="540">
   <si>
     <t>Running Delta Smelt Catch Data Collected for the USFWS Delta Smelt Experimental Release Technical Team</t>
   </si>
@@ -1665,6 +1665,21 @@
   </si>
   <si>
     <t>Cache Slough/LI</t>
+  </si>
+  <si>
+    <t>Lower Sacramento</t>
+  </si>
+  <si>
+    <t>24-41-LSR03</t>
+  </si>
+  <si>
+    <t>24-41-LSR05</t>
+  </si>
+  <si>
+    <t>24-41-SM11</t>
+  </si>
+  <si>
+    <t>24-41-LSR02</t>
   </si>
 </sst>
 </file>
@@ -2676,11 +2691,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
-  <dimension ref="A1:AE424"/>
+  <dimension ref="A1:AE429"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A392" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F423" sqref="F423"/>
+      <pane ySplit="1" topLeftCell="A419" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E434" sqref="E434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -25971,6 +25986,151 @@
         <v>-121.66952000000001</v>
       </c>
     </row>
+    <row r="425" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A425" s="44">
+        <v>45421</v>
+      </c>
+      <c r="B425" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C425" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D425" t="s">
+        <v>536</v>
+      </c>
+      <c r="E425" t="s">
+        <v>535</v>
+      </c>
+      <c r="J425">
+        <v>10</v>
+      </c>
+      <c r="K425" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L425">
+        <v>38.073219999999999</v>
+      </c>
+      <c r="M425">
+        <v>-121.76835</v>
+      </c>
+    </row>
+    <row r="426" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A426" s="44">
+        <v>45421</v>
+      </c>
+      <c r="B426" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C426" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D426" t="s">
+        <v>537</v>
+      </c>
+      <c r="E426" t="s">
+        <v>535</v>
+      </c>
+      <c r="J426">
+        <v>11.2</v>
+      </c>
+      <c r="K426" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L426">
+        <v>38.12433</v>
+      </c>
+      <c r="M426">
+        <v>-121.69927</v>
+      </c>
+    </row>
+    <row r="427" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A427" s="44">
+        <v>45421</v>
+      </c>
+      <c r="B427" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C427" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D427" t="s">
+        <v>537</v>
+      </c>
+      <c r="E427" t="s">
+        <v>535</v>
+      </c>
+      <c r="J427">
+        <v>7.5</v>
+      </c>
+      <c r="K427" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L427">
+        <v>38.12433</v>
+      </c>
+      <c r="M427">
+        <v>-121.69927</v>
+      </c>
+    </row>
+    <row r="428" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A428" s="44">
+        <v>45421</v>
+      </c>
+      <c r="B428" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C428" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D428" t="s">
+        <v>538</v>
+      </c>
+      <c r="E428" t="s">
+        <v>112</v>
+      </c>
+      <c r="J428">
+        <v>12.2</v>
+      </c>
+      <c r="K428" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L428">
+        <v>38.143770000000004</v>
+      </c>
+      <c r="M428">
+        <v>-122.06035</v>
+      </c>
+    </row>
+    <row r="429" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A429" s="44">
+        <v>45421</v>
+      </c>
+      <c r="B429" s="35" t="s">
+        <v>216</v>
+      </c>
+      <c r="C429" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="D429" t="s">
+        <v>539</v>
+      </c>
+      <c r="E429" t="s">
+        <v>535</v>
+      </c>
+      <c r="J429">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K429" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="L429">
+        <v>38.141530000000003</v>
+      </c>
+      <c r="M429">
+        <v>-121.69138</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AE254" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AE250">
@@ -25987,6 +26147,48 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e" xsi:nil="true"/>
+    <SharedWithUsers xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e">
+      <UserInfo>
+        <DisplayName>Hartman, Rosemary@DWR</DisplayName>
+        <AccountId>69</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Goodman, Denise M</DisplayName>
+        <AccountId>31</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Hobbs, James@Wildlife</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Cook, John (Ryan)</DisplayName>
+        <AccountId>18</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D9A9DE233A30CB4EAECD318FD55378CC" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8fd2cacec9171f93eb894d0689f08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="65146633-a755-433a-aacb-5024b6511b89" xmlns:ns3="d8e23be6-d007-4c2c-9265-7d9405abf22e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a569083f6831735b7a488ac820eb0384" ns2:_="" ns3:_="">
     <xsd:import namespace="65146633-a755-433a-aacb-5024b6511b89"/>
@@ -26221,49 +26423,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4F8AF6-B64B-4962-81B5-D73EE7A1E0CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
+    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="65146633-a755-433a-aacb-5024b6511b89">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e" xsi:nil="true"/>
-    <SharedWithUsers xmlns="d8e23be6-d007-4c2c-9265-7d9405abf22e">
-      <UserInfo>
-        <DisplayName>Hartman, Rosemary@DWR</DisplayName>
-        <AccountId>69</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Goodman, Denise M</DisplayName>
-        <AccountId>31</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Hobbs, James@Wildlife</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Cook, John (Ryan)</DisplayName>
-        <AccountId>18</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76D96E8C-3FF7-4769-9DB8-E43AB53278F6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26280,23 +26459,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E7C764E5-19B4-4012-98BF-B46F2FA7A2CF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D4F8AF6-B64B-4962-81B5-D73EE7A1E0CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="65146633-a755-433a-aacb-5024b6511b89"/>
-    <ds:schemaRef ds:uri="d8e23be6-d007-4c2c-9265-7d9405abf22e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Dec 4th 2024 update
</commit_message>
<xml_diff>
--- a/Running Delta Smelt Catch_2023-09-05.xlsx
+++ b/Running Delta Smelt Catch_2023-09-05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/SmeltMap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="8_{38D2B3C1-DAF9-4126-B4FD-0E27163FBC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFC90DD8-1D19-45F2-B7BC-44975BEE048E}"/>
+  <xr:revisionPtr revIDLastSave="201" documentId="8_{38D2B3C1-DAF9-4126-B4FD-0E27163FBC27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9B4164F-1224-45A6-BEDD-07D8A0A4A2DC}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{4BB403AD-DB3F-4CB5-B7F1-39827ED458E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="12" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6226" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6244" uniqueCount="580">
   <si>
     <t>Running Delta Smelt Catch Data Collected for the USFWS Delta Smelt Experimental Release Technical Team</t>
   </si>
@@ -1786,14 +1786,30 @@
   </si>
   <si>
     <t>25-16-SM03</t>
+  </si>
+  <si>
+    <t>25-18-SSC05</t>
+  </si>
+  <si>
+    <t>VIE-LBA</t>
+  </si>
+  <si>
+    <t>Lookout Slough</t>
+  </si>
+  <si>
+    <t>BY2024 1</t>
+  </si>
+  <si>
+    <t>25-18-CS10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1974,7 +1990,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2092,6 +2108,7 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2803,11 +2820,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C569B310-60E0-4E31-89EB-52CC1C810311}">
-  <dimension ref="A1:AE504"/>
+  <dimension ref="A1:AE506"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A486" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F506" sqref="F506"/>
+      <pane ySplit="1" topLeftCell="A493" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S513" sqref="S513"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -31975,6 +31992,94 @@
       </c>
       <c r="V504" s="14" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="505" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A505" s="48">
+        <v>45621</v>
+      </c>
+      <c r="B505" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C505" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D505" t="s">
+        <v>575</v>
+      </c>
+      <c r="E505" t="s">
+        <v>533</v>
+      </c>
+      <c r="J505">
+        <v>64</v>
+      </c>
+      <c r="K505" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="L505" s="49">
+        <v>38.462179999999996</v>
+      </c>
+      <c r="M505" s="49">
+        <v>-121.58891</v>
+      </c>
+      <c r="R505" t="s">
+        <v>576</v>
+      </c>
+      <c r="S505" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="T505" s="21">
+        <v>45614</v>
+      </c>
+      <c r="U505" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="V505" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="506" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A506" s="21">
+        <v>45623</v>
+      </c>
+      <c r="B506" s="14" t="s">
+        <v>216</v>
+      </c>
+      <c r="C506" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="D506" t="s">
+        <v>579</v>
+      </c>
+      <c r="E506" t="s">
+        <v>76</v>
+      </c>
+      <c r="J506" s="14">
+        <v>62</v>
+      </c>
+      <c r="K506" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="L506" s="49">
+        <v>38.24156</v>
+      </c>
+      <c r="M506" s="49">
+        <v>-121.68801999999999</v>
+      </c>
+      <c r="R506" t="s">
+        <v>576</v>
+      </c>
+      <c r="S506" s="14" t="s">
+        <v>578</v>
+      </c>
+      <c r="T506" s="21">
+        <v>45614</v>
+      </c>
+      <c r="U506" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="V506" s="14" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>